<commit_message>
ajustes carga e leiaute
</commit_message>
<xml_diff>
--- a/dados/propostas_mon/relatorio_propostas.xlsx
+++ b/dados/propostas_mon/relatorio_propostas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="251">
   <si>
     <t>Nº da Proposta</t>
   </si>
@@ -580,6 +580,48 @@
     <t>24/05/2023</t>
   </si>
   <si>
+    <t>170512</t>
+  </si>
+  <si>
+    <t>13.849.028/0001-40</t>
+  </si>
+  <si>
+    <t>FUNDO ESTADUAL DE SAUDE DO TOCANTINS</t>
+  </si>
+  <si>
+    <t>PALMAS</t>
+  </si>
+  <si>
+    <t>TO</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>ABREULANDIA; AGUIARNOPOLIS; ALIANCA DO TOCANTINS; ALMAS; ALVORADA; ANANAS; ANGICO; APARECIDA DO RIO NEGRO; ARAGOMINAS; ARAGUACEMA; ARAGUACU; ARAGUAINA; ARAGUANA; ARAGUATINS; ARAPOEMA; ARRAIAS; AUGUSTINOPOLIS; AURORA DO TOCANTINS; AXIXA DO TOCANTINS; BABACULANDIA; BANDEIRANTES DO TOCANTINS; BARRA DO OURO; BARROLANDIA; BERNARDO SAYAO; BOM JESUS DO TOCANTINS; BRASILANDIA DO TOCANTINS; BREJINHO DE NAZARE; BURITI DO TOCANTINS; CACHOEIRINHA; CAMPOS LINDOS; CARIRI DO TOCANTINS; CARMOLANDIA; CARRASCO BONITO; CASEARA; CENTENARIO; CHAPADA DE AREIA; CHAPADA DA NATIVIDADE; COLINAS DO TOCANTINS; COMBINADO; CONCEICAO DO TOCANTINS; COUTO MAGALHAES; CRISTALANDIA; CRIXAS DO TOCANTINS; DARCINOPOLIS; DIANOPOLIS; DIVINOPOLIS DO TOCANTINS; DOIS IRMAOS DO TOCANTINS; DUERE; ESPERANTINA; FATIMA; FIGUEIROPOLIS; FILADELFIA; FORMOSO DO ARAGUAIA; FORTALEZA DO TABOCAO; GOIANORTE; GOIATINS; GUARAI; GURUPI; IPUEIRAS; ITACAJA; ITAGUATINS; ITAPIRATINS; ITAPORA DO TOCANTINS; JAU DO TOCANTINS; JUARINA; LAGOA DA CONFUSAO; LAGOA DO TOCANTINS; LAJEADO; LAVANDEIRA; LIZARDA; LUZINOPOLIS; MARIANOPOLIS DO TOCANTINS; MATEIROS; MAURILANDIA DO TOCANTINS; MIRACEMA DO TOCANTINS; MIRANORTE; MONTE DO CARMO; MONTE SANTO DO TOCANTINS; PALMEIRAS DO TOCANTINS; MURICILANDIA; NATIVIDADE; NAZARE; NOVA OLINDA; NOVA ROSALANDIA; NOVO ACORDO; NOVO ALEGRE; NOVO JARDIM; OLIVEIRA DE FATIMA; PALMEIRANTE; PALMEIROPOLIS; PARAISO DO TOCANTINS; PARANA; PAU D'ARCO; PEDRO AFONSO; PEIXE; PEQUIZEIRO; COLMEIA; PINDORAMA DO TOCANTINS; PIRAQUE; PIUM; PONTE ALTA DO BOM JESUS; PONTE ALTA DO TOCANTINS; PORTO ALEGRE DO TOCANTINS; PORTO NACIONAL; PRAIA NORTE; PRESIDENTE KENNEDY; PUGMIL; RECURSOLANDIA; RIACHINHO; RIO DA CONCEICAO; RIO DOS BOIS; RIO SONO; SAMPAIO; SANDOLANDIA; SANTA FE DO ARAGUAIA; SANTA MARIA DO TOCANTINS; SANTA RITA DO TOCANTINS; SANTA ROSA DO TOCANTINS; SANTA TEREZA DO TOCANTINS; SANTA TEREZINHA DO TOCANTINS; SAO BENTO DO TOCANTINS; SAO FELIX DO TOCANTINS; SAO MIGUEL DO TOCANTINS; SAO SALVADOR DO TOCANTINS; SAO SEBASTIAO DO TOCANTINS; SAO VALERIO; SILVANOPOLIS; SITIO NOVO DO TOCANTINS; SUCUPIRA; TAGUATINGA; TAIPAS DO TOCANTINS; TALISMA; PALMAS; TOCANTINIA; TOCANTINOPOLIS; TUPIRAMA; TUPIRATINS; WANDERLANDIA; XAMBIOA</t>
+  </si>
+  <si>
+    <t>170025; 170030; 170035; 170040; 170070; 170100; 170105; 170110; 170130; 170190; 170200; 170210; 170215; 170220; 170230; 170240; 170255; 170270; 170290; 170300; 170305; 170307; 170310; 170320; 170330; 170360; 170370; 170380; 170382; 170384; 170386; 170388; 170389; 170390; 170410; 170460; 170510; 170550; 170555; 170560; 170600; 170610; 170625; 170650; 170700; 170710; 170720; 170730; 170740; 170755; 170765; 170770; 170820; 170825; 170830; 170900; 170930; 170950; 170980; 171050; 171070; 171090; 171110; 171150; 171180; 171190; 171195; 171200; 171215; 171240; 171245; 171250; 171270; 171280; 171320; 171330; 171360; 171370; 171380; 171395; 171420; 171430; 171488; 171500; 171510; 171515; 171525; 171550; 171570; 171575; 171610; 171620; 171630; 171650; 171660; 171665; 171670; 171700; 171720; 171750; 171780; 171790; 171800; 171820; 171830; 171840; 171845; 171850; 171855; 171865; 171870; 171875; 171880; 171884; 171886; 171888; 171889; 171890; 171900; 172000; 172010; 172015; 172020; 172025; 172030; 172049; 172065; 172080; 172085; 172090; 172093; 172097; 172100; 172110; 172120; 172125; 172130; 172208; 172210</t>
+  </si>
+  <si>
+    <t>1607363</t>
+  </si>
+  <si>
+    <t>JULIANA RIBEIRO PINTO</t>
+  </si>
+  <si>
+    <t>juenf86@gmail.com</t>
+  </si>
+  <si>
+    <t>61 86119188</t>
+  </si>
+  <si>
+    <t>24/02/2023</t>
+  </si>
+  <si>
+    <t>25/05/2023</t>
+  </si>
+  <si>
     <t>170520</t>
   </si>
   <si>
@@ -614,12 +656,6 @@
   </si>
   <si>
     <t>21 23334031</t>
-  </si>
-  <si>
-    <t>24/02/2023</t>
-  </si>
-  <si>
-    <t>25/05/2023</t>
   </si>
   <si>
     <t>Laura Vanessa de Souza Albuquerque</t>
@@ -637,6 +673,113 @@
 marcelo.rodrigues@saude.rj.gov.br
 marcelo.rodrigues.castro@gmail.com
 laura.albuquerque@saude.rj.gov.br</t>
+  </si>
+  <si>
+    <t>170522</t>
+  </si>
+  <si>
+    <t>74.031.865/0001-51</t>
+  </si>
+  <si>
+    <t>FORTALEZA</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>Mutirão de cirurgias eletivas. Tem como objetivos: organizar e ampliar o acesso a cirurgias, exames e consultas na Atenção Especializada à 
+Saúde, em especial àqueles com demanda reprimida identificada, aprimorar a governança da Rede de Atenção à Saúde com centralidade na garantia do acesso, gestão por resultados e financiamento estável; fomentar o monitoramento e a avaliação das ações e dos serviços de saúde, visando melhorar a qualidade da atenção especializada e ampliar o acesso à saúde; qualificar a contratualização com a rede complementar; mudar modelo de gestão e regulação das filas para a atenção especializada (regulação do acesso), visando a adequar a oferta de ações e serviços de saúde de acordo com as necessidades de saúde, estratificação de risco e necessidades assistenciais e fomentar a implementação de um novo modelo de custeio para a atenção ambulatorial especializada e para a realização de cirurgias eletivas.</t>
+  </si>
+  <si>
+    <t>ABAIARA; ACARAPE; ACARAU; ACOPIARA; AIUABA; ALCANTARAS; ALTANEIRA; ALTO SANTO; AMONTADA; ANTONINA DO NORTE; APUIARES; AQUIRAZ; ARACATI; ARACOIABA; ARARENDA; ARARIPE; ARATUBA; ARNEIROZ; ASSARE; AURORA; BAIXIO; BANABUIU; BARBALHA; BARREIRA; BARRO; BARROQUINHA; BATURITE; BEBERIBE; BELA CRUZ; BOA VIAGEM; BREJO SANTO; CAMOCIM; CAMPOS SALES; CANINDE; CAPISTRANO; CARIDADE; CARIRE; CARIRIACU; CARIUS; CARNAUBAL; CASCAVEL; CATARINA; CATUNDA; CAUCAIA; CEDRO; CHAVAL; CHORO; CHOROZINHO; COREAU; CRATEUS; CRATO; CROATA; CRUZ; DEPUTADO IRAPUAN PINHEIRO; ERERE; EUSEBIO; FARIAS BRITO; FORQUILHA; FORTALEZA; FORTIM; FRECHEIRINHA; GENERAL SAMPAIO; GRACA; GRANJA; GRANJEIRO; GROAIRAS; GUAIUBA; GUARACIABA DO NORTE; GUARAMIRANGA; HIDROLANDIA; HORIZONTE; IBARETAMA; IBIAPINA; IBICUITINGA; ICAPUI; ICO; IGUATU; INDEPENDENCIA; IPAPORANGA; IPAUMIRIM; IPU; IPUEIRAS; IRACEMA; IRAUCUBA; ITAICABA; ITAITINGA; ITAPAGE; ITAPIPOCA; ITAPIUNA; ITAREMA; ITATIRA; JAGUARETAMA; JAGUARIBARA; JAGUARIBE; JAGUARUANA; JARDIM; JATI; JIJOCA DE JERICOACOARA; JUAZEIRO DO NORTE; JUCAS; LAVRAS DA MANGABEIRA; LIMOEIRO DO NORTE; MADALENA; MARACANAU; MARANGUAPE; MARCO; MARTINOPOLE; MASSAPE; MAURITI; MERUOCA; MILAGRES; MILHA; MIRAIMA; MISSAO VELHA; MOMBACA; MONSENHOR TABOSA; MORADA NOVA; MORAUJO; MORRINHOS; MUCAMBO; MULUNGU; NOVA OLINDA; NOVA RUSSAS; NOVO ORIENTE; OCARA; OROS; PACAJUS; PACATUBA; PACOTI; PACUJA; PALHANO; PALMACIA; PARACURU; PARAIPABA; PARAMBU; PARAMOTI; PEDRA BRANCA; PENAFORTE; PENTECOSTE; PEREIRO; PINDORETAMA; PIQUET CARNEIRO; PIRES FERREIRA; PORANGA; PORTEIRAS; POTENGI; POTIRETAMA; QUITERIANOPOLIS; QUIXADA; QUIXELO; QUIXERAMOBIM; QUIXERE; REDENCAO; RERIUTABA; RUSSAS; SABOEIRO; SALITRE; SANTANA DO ACARAU; SANTANA DO CARIRI; SANTA QUITERIA; SAO BENEDITO; SAO GONCALO DO AMARANTE; SAO JOAO DO JAGUARIBE; SAO LUIS DO CURU; SENADOR POMPEU; SENADOR SA; SOBRAL; SOLONOPOLE; TABULEIRO DO NORTE; TAMBORIL; TARRAFAS; TAUA; TEJUCUOCA; TIANGUA; TRAIRI; TURURU; UBAJARA; UMARI; UMIRIM; URUBURETAMA; URUOCA; VARJOTA; VARZEA ALEGRE; VICOSA DO CEARA</t>
+  </si>
+  <si>
+    <t>230010; 230015; 230020; 230030; 230040; 230050; 230060; 230070; 230075; 230080; 230090; 230100; 230110; 230120; 230125; 230130; 230140; 230150; 230160; 230170; 230180; 230185; 230190; 230195; 230200; 230205; 230210; 230220; 230230; 230240; 230250; 230260; 230270; 230280; 230290; 230300; 230310; 230320; 230330; 230340; 230350; 230360; 230365; 230370; 230380; 230390; 230393; 230395; 230400; 230410; 230420; 230423; 230425; 230426; 230427; 230428; 230430; 230435; 230440; 230445; 230450; 230460; 230465; 230470; 230480; 230490; 230495; 230500; 230510; 230520; 230523; 230526; 230530; 230533; 230535; 230540; 230550; 230560; 230565; 230570; 230580; 230590; 230600; 230610; 230620; 230625; 230630; 230640; 230650; 230655; 230660; 230670; 230680; 230690; 230700; 230710; 230720; 230725; 230730; 230740; 230750; 230760; 230763; 230765; 230770; 230780; 230790; 230800; 230810; 230820; 230830; 230835; 230837; 230840; 230850; 230860; 230870; 230880; 230890; 230900; 230910; 230920; 230930; 230940; 230945; 230950; 230960; 230970; 230980; 230990; 231000; 231010; 231020; 231025; 231030; 231040; 231050; 231060; 231070; 231080; 231085; 231090; 231095; 231100; 231110; 231120; 231123; 231126; 231130; 231135; 231140; 231150; 231160; 231170; 231180; 231190; 231195; 231200; 231210; 231220; 231230; 231240; 231250; 231260; 231270; 231280; 231290; 231300; 231310; 231320; 231325; 231330; 231335; 231340; 231350; 231355; 231360; 231370; 231375; 231380; 231390; 231395; 231400; 231410</t>
+  </si>
+  <si>
+    <t>9240580</t>
+  </si>
+  <si>
+    <t>25.991.043,34</t>
+  </si>
+  <si>
+    <t>QUELVIA DA SILVA LIMA</t>
+  </si>
+  <si>
+    <t>quelviaadm@gmail.com</t>
+  </si>
+  <si>
+    <t>85 99657881</t>
+  </si>
+  <si>
+    <t>170537</t>
+  </si>
+  <si>
+    <t>06.023.953/0001-51</t>
+  </si>
+  <si>
+    <t>ESTADO DO MARANHAO - FUNDO ESTADUAL DE SAUDE / FES</t>
+  </si>
+  <si>
+    <t>SAO LUIS</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>ACAILANDIA; AFONSO CUNHA; AGUA DOCE DO MARANHAO; ALCANTARA; ALDEIAS ALTAS; ALTAMIRA DO MARANHAO; ALTO ALEGRE DO MARANHAO; ALTO ALEGRE DO PINDARE; ALTO PARNAIBA; AMAPA DO MARANHAO; AMARANTE DO MARANHAO; ANAJATUBA; ANAPURUS; APICUM-ACU; ARAGUANA; ARAIOSES; ARAME; ARARI; AXIXA; BACABAL; BACABEIRA; BACURI; BACURITUBA; BALSAS; BARAO DE GRAJAU; BARRA DO CORDA; BARREIRINHAS; BELAGUA; BELA VISTA DO MARANHAO; BENEDITO LEITE; BEQUIMAO; BERNARDO DO MEARIM; BOA VISTA DO GURUPI; BOM JARDIM; BOM JESUS DAS SELVAS; BOM LUGAR; BREJO; BREJO DE AREIA; BURITI; BURITI BRAVO; BURITICUPU; BURITIRANA; CACHOEIRA GRANDE; CAJAPIO; CAJARI; CAMPESTRE DO MARANHAO; CANDIDO MENDES; CANTANHEDE; CAPINZAL DO NORTE; CAROLINA; CARUTAPERA; CAXIAS; CEDRAL; CENTRAL DO MARANHAO; CENTRO DO GUILHERME; CENTRO NOVO DO MARANHAO; CHAPADINHA; CIDELANDIA; CODO; COELHO NETO; COLINAS; CONCEICAO DO LAGO-ACU; COROATA; CURURUPU; DAVINOPOLIS; DOM PEDRO; DUQUE BACELAR; ESPERANTINOPOLIS; ESTREITO; FEIRA NOVA DO MARANHAO; FERNANDO FALCAO; FORMOSA DA SERRA NEGRA; FORTALEZA DOS NOGUEIRAS; FORTUNA; GODOFREDO VIANA; GONCALVES DIAS; GOVERNADOR ARCHER; GOVERNADOR EDISON LOBAO; GOVERNADOR EUGENIO BARROS; GOVERNADOR LUIZ ROCHA; GOVERNADOR NEWTON BELLO; GOVERNADOR NUNES FREIRE; GRACA ARANHA; GRAJAU; GUIMARAES; HUMBERTO DE CAMPOS; ICATU; IGARAPE DO MEIO; IGARAPE GRANDE; IMPERATRIZ; ITAIPAVA DO GRAJAU; ITAPECURU MIRIM; ITINGA DO MARANHAO; JATOBA; JENIPAPO DOS VIEIRAS; JOAO LISBOA; JOSELANDIA; JUNCO DO MARANHAO; LAGO DA PEDRA; LAGO DO JUNCO; LAGO VERDE; LAGOA DO MATO; LAGO DOS RODRIGUES; LAGOA GRANDE DO MARANHAO; LAJEADO NOVO; LIMA CAMPOS; LORETO; LUIS DOMINGUES; MAGALHAES DE ALMEIDA; MARACACUME; MARAJA DO SENA; MARANHAOZINHO; MATA ROMA; MATINHA; MATOES; MATOES DO NORTE; MILAGRES DO MARANHAO; MIRADOR; MIRANDA DO NORTE; MIRINZAL; MONCAO; MONTES ALTOS; MORROS; NINA RODRIGUES; NOVA COLINAS; NOVA IORQUE; NOVA OLINDA DO MARANHAO; OLHO D'AGUA DAS CUNHAS; OLINDA NOVA DO MARANHAO; PACO DO LUMIAR; PALMEIRANDIA; PARAIBANO; PARNARAMA; PASSAGEM FRANCA; PASTOS BONS; PAULINO NEVES; PAULO RAMOS; PEDREIRAS; PEDRO DO ROSARIO; PENALVA; PERI MIRIM; PERITORO; PINDARE-MIRIM; PINHEIRO; PIO XII; PIRAPEMAS; POCAO DE PEDRAS; PORTO FRANCO; PORTO RICO DO MARANHAO; PRESIDENTE DUTRA; PRESIDENTE JUSCELINO; PRESIDENTE MEDICI; PRESIDENTE SARNEY; PRESIDENTE VARGAS; PRIMEIRA CRUZ; RAPOSA; RIACHAO; RIBAMAR FIQUENE; ROSARIO; SAMBAIBA; SANTA FILOMENA DO MARANHAO; SANTA HELENA; SANTA INES; SANTA LUZIA; SANTA LUZIA DO PARUA; SANTA QUITERIA DO MARANHAO; SANTA RITA; SANTANA DO MARANHAO; SANTO AMARO DO MARANHAO; SANTO ANTONIO DOS LOPES; SAO BENEDITO DO RIO PRETO; SAO BENTO; SAO BERNARDO; SAO DOMINGOS DO AZEITAO; SAO DOMINGOS DO MARANHAO; SAO FELIX DE BALSAS; SAO FRANCISCO DO BREJAO; SAO FRANCISCO DO MARANHAO; SAO JOAO BATISTA; SAO JOAO DO CARU; SAO JOAO DO PARAISO; SAO JOAO DO SOTER; SAO JOAO DOS PATOS; SAO JOSE DE RIBAMAR; SAO JOSE DOS BASILIOS; SAO LUIS; SAO LUIS GONZAGA DO MARANHAO; SAO MATEUS DO MARANHAO; SAO PEDRO DA AGUA BRANCA; SAO PEDRO DOS CRENTES; SAO RAIMUNDO DAS MANGABEIRAS; SAO RAIMUNDO DO DOCA BEZERRA; SAO ROBERTO; SAO VICENTE FERRER; SATUBINHA; SENADOR ALEXANDRE COSTA; SENADOR LA ROCQUE; SERRANO DO MARANHAO; SITIO NOVO; SUCUPIRA DO NORTE; SUCUPIRA DO RIACHAO; TASSO FRAGOSO; TIMBIRAS; TIMON; TRIZIDELA DO VALE; TUFILANDIA; TUNTUM; TURIACU; TURILANDIA; TUTOIA; URBANO SANTOS; VARGEM GRANDE; VIANA; VILA NOVA DOS MARTIRIOS; VITORIA DO MEARIM; VITORINO FREIRE; ZE DOCA</t>
+  </si>
+  <si>
+    <t>210005; 210010; 210015; 210020; 210030; 210040; 210043; 210047; 210050; 210055; 210060; 210070; 210080; 210083; 210087; 210090; 210095; 210100; 210110; 210120; 210125; 210130; 210135; 210140; 210150; 210160; 210170; 210173; 210177; 210180; 210190; 210193; 210197; 210200; 210203; 210207; 210210; 210215; 210220; 210230; 210232; 210235; 210237; 210240; 210250; 210255; 210260; 210270; 210275; 210280; 210290; 210300; 210310; 210312; 210315; 210317; 210320; 210325; 210330; 210340; 210350; 210355; 210360; 210370; 210375; 210380; 210390; 210400; 210405; 210407; 210408; 210409; 210410; 210420; 210430; 210440; 210450; 210455; 210460; 210462; 210465; 210467; 210470; 210480; 210490; 210500; 210510; 210515; 210520; 210530; 210535; 210540; 210542; 210545; 210547; 210550; 210560; 210565; 210570; 210580; 210590; 210592; 210594; 210596; 210598; 210600; 210610; 210620; 210630; 210632; 210635; 210637; 210640; 210650; 210660; 210663; 210667; 210670; 210675; 210680; 210690; 210700; 210710; 210720; 210725; 210730; 210735; 210740; 210745; 210750; 210760; 210770; 210780; 210790; 210800; 210805; 210810; 210820; 210825; 210830; 210840; 210845; 210850; 210860; 210870; 210880; 210890; 210900; 210905; 210910; 210920; 210923; 210927; 210930; 210940; 210945; 210950; 210955; 210960; 210970; 210975; 210980; 210990; 211000; 211003; 211010; 211020; 211023; 211027; 211030; 211040; 211050; 211060; 211065; 211070; 211080; 211085; 211090; 211100; 211102; 211105; 211107; 211110; 211120; 211125; 211130; 211140; 211150; 211153; 211157; 211160; 211163; 211167; 211170; 211172; 211174; 211176; 211178; 211180; 211190; 211195; 211200; 211210; 211220; 211223; 211227; 211230; 211240; 211245; 211250; 211260; 211270; 211280; 211285; 211290; 211300; 211400</t>
+  </si>
+  <si>
+    <t>7153262</t>
+  </si>
+  <si>
+    <t>20.120.029,55</t>
+  </si>
+  <si>
+    <t>LUCIANA AMORIM TOMICH NETTO GUTERRES SOARES</t>
+  </si>
+  <si>
+    <t>lucianatomich@yahoo.com.br</t>
+  </si>
+  <si>
+    <t>98 99143176</t>
+  </si>
+  <si>
+    <t>27/02/2023</t>
+  </si>
+  <si>
+    <t>28/05/2023</t>
+  </si>
+  <si>
+    <t>Marina Nascimento Sousa</t>
+  </si>
+  <si>
+    <t>Superintendência de Avaliação e Controle do Sistema de Saúde/SES</t>
+  </si>
+  <si>
+    <t>(98) 98127-8774</t>
+  </si>
+  <si>
+    <t>marinasousa20@gmail.com</t>
+  </si>
+  <si>
+    <t>Há uma demanda reprimida para procedimentos cirúrgicos eletivos de media e alta complexidade, potencializada pela Pandemia Covid 19. A Secretaria de Estado da Saúde do Maranhão em conjunto com os municípios descentralizou os serviços de saúde ambulatoriais e hospitalares para as 19 Regiões de Saúde, abrangendo os 217 municípios maranhenses. Desta feita, os procedimentos cirúrgicos eletivos serão realizados nos estabelecimentos de saúde de gestão estadual e municipal</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Para ampliação dos serviços será necessário implementar os serviços nos estabelecimentos de saude adotando as seguintes medidas:
+* Aumento da capacidade de atendiemnto dos serviços de saude no ambito ambulatorial e hospitalar;
+* Melhor utilização da capacidade dos Serviços implementando o sistema de produtividade;
+* Ampliação de turno de trabalho para os procedimentos a serem realizados;
+* Ampliação das equipes multiprofissionais de saúde para a realização dos procedimentos cirúrgicos.</t>
+  </si>
+  <si>
+    <t>A gestão da fila cirúrgica será realizada pela gestão estadual com sistema de compartilhamento com os municípios, visando o acompanhamento das metas programadas e realizadas por cada estabelecimento de saúde e cronograma de execução estabelecido no Plano Nacional de Redução de Filas</t>
   </si>
 </sst>
 </file>
@@ -1010,10 +1153,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BY10"/>
+  <dimension ref="A1:BY13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="BY10" sqref="BY10"/>
+      <selection activeCell="BY13" sqref="BY13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3349,81 +3492,780 @@
         <v>79</v>
       </c>
       <c r="AZ10" s="2" t="s">
-        <v>191</v>
+        <v>79</v>
       </c>
       <c r="BA10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BB10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BC10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BD10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BE10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BF10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BH10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BK10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BL10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BN10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BP10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BQ10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BR10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BS10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BT10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BU10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BV10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BW10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BX10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BY10" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:77">
+      <c r="A11" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="BB10" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="BC10" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="BD10" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="BE10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BF10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BG10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BH10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BI10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BJ10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BK10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BL10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BM10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BN10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BO10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BP10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BQ10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BR10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BS10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BT10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BU10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BV10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BW10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BX10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BY10" s="2" t="s">
+      <c r="K11" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR11" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="AS11" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="AT11" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="AU11" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AV11" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AW11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ11" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="BA11" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="BB11" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="BC11" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="BD11" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="BE11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BF11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BH11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BK11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BL11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BN11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BP11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BQ11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BR11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BS11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BT11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BU11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BV11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BW11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BX11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BY11" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:77">
+      <c r="A12" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD12" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="AE12" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="AF12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR12" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="AS12" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="AT12" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU12" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AV12" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AW12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BB12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BC12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BD12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BE12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BF12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BH12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BK12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BL12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BN12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BP12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BQ12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BR12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BS12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BT12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BU12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BV12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BW12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BX12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BY12" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:77">
+      <c r="A13" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD13" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE13" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR13" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="AS13" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="AT13" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="AU13" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="AV13" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="AW13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ13" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="BA13" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="BB13" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="BC13" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="BD13" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="BE13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BF13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG13" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="BH13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BJ13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BK13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BL13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BM13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BN13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BO13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BP13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BQ13" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="BR13" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="BS13" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="BT13" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="BU13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BV13" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="BW13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BX13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BY13" s="2" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ajustes para maior fluidez em dispositivos móveis
</commit_message>
<xml_diff>
--- a/dados/propostas_mon/relatorio_propostas.xlsx
+++ b/dados/propostas_mon/relatorio_propostas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="345">
   <si>
     <t>Nº da Proposta</t>
   </si>
@@ -457,6 +457,9 @@
     <t>Sim</t>
   </si>
   <si>
+    <t>Não</t>
+  </si>
+  <si>
     <t>170358</t>
   </si>
   <si>
@@ -580,6 +583,64 @@
     <t>24/05/2023</t>
   </si>
   <si>
+    <t>170506</t>
+  </si>
+  <si>
+    <t>04.384.829/0001-96</t>
+  </si>
+  <si>
+    <t>ARACAJU</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>Considerando que a saúde é um direito fundamental do ser humano, devendo o Estado prover as condições indispensáveis ao seu pleno exercício, Art. 2º da Lei nº 8.080, de 19 de setembro de 1990, que dispõe sobre as condições para a promoção, proteção e recuperação da saúde, a organização e o funcionamento dos serviços correspondentes e dá outras providências;
+	Considerando a Portaria n o 4.279, de 30 de dezembro de 2010, que estabelece diretrizes para a organização da Rede de Atenção à Saúde no âmbito do Sistema Único de Saúde;
+	Considerando a Relação Nacional de Ações e Serviços de Saúde RENASES, que compreende todas as ações e serviços que o Sistema Único de Saúde - SUS oferece ao usuário, para atendimento da integralidade da assistência à saúde, em atendimento ao disposto no art. 22, do Decreto n o 7.508, de 28 de junho de 2011 e no art. 70, inciso II, da Lei 8.080/90;
+	Considerando a Portaria n o 3.390, de 30 de dezembro de 2013, que institui a Política Nacional de Atenção Hospitalar (PNHOSP) no âmbito do Sistema Único de Saúde (SUS), estabelecendo as diretrizes para a organização do componente hospitalar da Rede de Atenção à Saúde (RAS);
+Considerando as diretrizes para a Contratualização de hospitais no âmbito do Sistema Único de Saúde;
+	Considerando que o Estado de Sergipe, atualmente, possui uma fila de  pacientes aguardando a realização de Cirurgias Eletivas em diversas especialidades como cirurgia geral, ortopedia, oftalmologia, otorrinolaringologia, cardiologia, neurocirurgia e outras; 
+	Considerando a necessidade em ofertar serviços de saúde, garantindo o acesso ao atendimento dos pacientes do SUS, em sintonia com as necessidades de saúde da população, com as políticas públicas de saúde para atenção hospitalar e com os princípios e diretrizes do SUS;
+	Considerando o compromisso em atender a demanda dos usuários do SUS Sergipe, residentes nos 75 municípios do Estado, com demanda pela realização de procedimentos cirúrgicos eletivos de média e alta complexidade; 
+Considerando a Portaria GM/MS nº 90, de 03 de fevereiro de 2023, que institui o Programa Nacional de Redução das Filas de CirurgiasEletivas, Exames Complementares e Consultas Especializadas.
+	 Diante do exposto, justifica-se a elaboração do Plano Estadual de Redução de Filas de Cirurgias Eletivas, em especial àquelas com demanda reprimida identificada, no Estado de Sergipe, conforme procedimentos descritos na Tabela de Procedimentos, Medicamentos, Órteses e Próteses e Materiais Especiais (OPM) do Sistema Único de Saúde ¿ SUS, e constante nos documentos em anexos.</t>
+  </si>
+  <si>
+    <t>AMPARO DE SAO FRANCISCO; AQUIDABA; ARACAJU; ARAUA; AREIA BRANCA; BARRA DOS COQUEIROS; BOQUIM; BREJO GRANDE; CAMPO DO BRITO; CANHOBA; CANINDE DE SAO FRANCISCO; CAPELA; CARIRA; CARMOPOLIS; CEDRO DE SAO JOAO; CRISTINAPOLIS; CUMBE; DIVINA PASTORA; ESTANCIA; FEIRA NOVA; FREI PAULO; GARARU; GENERAL MAYNARD; GRACHO CARDOSO; ILHA DAS FLORES; INDIAROBA; ITABAIANA; ITABAIANINHA; ITABI; ITAPORANGA D'AJUDA; JAPARATUBA; JAPOATA; LAGARTO; LARANJEIRAS; MACAMBIRA; MALHADA DOS BOIS; MALHADOR; MARUIM; MOITA BONITA; MONTE ALEGRE DE SERGIPE; MURIBECA; NEOPOLIS; NOSSA SENHORA APARECIDA; NOSSA SENHORA DA GLORIA; NOSSA SENHORA DAS DORES; NOSSA SENHORA DE LOURDES; NOSSA SENHORA DO SOCORRO; PACATUBA; PEDRA MOLE; PEDRINHAS; PINHAO; PIRAMBU; POCO REDONDO; POCO VERDE; PORTO DA FOLHA; PROPRIA; RIACHAO DO DANTAS; RIACHUELO; RIBEIROPOLIS; ROSARIO DO CATETE; SALGADO; SANTA LUZIA DO ITANHY; SANTANA DO SAO FRANCISCO; SANTA ROSA DE LIMA; SANTO AMARO DAS BROTAS; SAO CRISTOVAO; SAO DOMINGOS; SAO FRANCISCO; SAO MIGUEL DO ALEIXO; SIMAO DIAS; SIRIRI; TELHA; TOBIAS BARRETO; TOMAR DO GERU; UMBAUBA</t>
+  </si>
+  <si>
+    <t>280010; 280020; 280030; 280040; 280050; 280060; 280067; 280070; 280100; 280110; 280120; 280130; 280140; 280150; 280160; 280170; 280190; 280200; 280210; 280220; 280230; 280240; 280250; 280260; 280270; 280280; 280290; 280300; 280310; 280320; 280330; 280340; 280350; 280360; 280370; 280380; 280390; 280400; 280410; 280420; 280430; 280440; 280445; 280450; 280460; 280470; 280480; 280490; 280500; 280510; 280520; 280530; 280540; 280550; 280560; 280570; 280580; 280590; 280600; 280610; 280620; 280630; 280640; 280650; 280660; 280670; 280680; 280690; 280700; 280710; 280720; 280730; 280740; 280750; 280760</t>
+  </si>
+  <si>
+    <t>2338474</t>
+  </si>
+  <si>
+    <t>NEUZICE OLIVEIRA LIMA</t>
+  </si>
+  <si>
+    <t>neuzice.lima@saude.se.gov.br</t>
+  </si>
+  <si>
+    <t>79 32268375</t>
+  </si>
+  <si>
+    <t>24/02/2023</t>
+  </si>
+  <si>
+    <t>25/05/2023</t>
+  </si>
+  <si>
+    <t>Neuzice Oliveira Lima</t>
+  </si>
+  <si>
+    <t>Coordenadora Estadual de Articulação de Redes Temáticas.</t>
+  </si>
+  <si>
+    <t>(79) 3226-8375
+(79) 99922-1799</t>
+  </si>
+  <si>
     <t>170512</t>
   </si>
   <si>
@@ -614,12 +675,6 @@
   </si>
   <si>
     <t>61 86119188</t>
-  </si>
-  <si>
-    <t>24/02/2023</t>
-  </si>
-  <si>
-    <t>25/05/2023</t>
   </si>
   <si>
     <t>170520</t>
@@ -727,13 +782,19 @@
     <t>MA</t>
   </si>
   <si>
-    <t>ACAILANDIA; AFONSO CUNHA; AGUA DOCE DO MARANHAO; ALCANTARA; ALDEIAS ALTAS; ALTAMIRA DO MARANHAO; ALTO ALEGRE DO MARANHAO; ALTO ALEGRE DO PINDARE; ALTO PARNAIBA; AMAPA DO MARANHAO; AMARANTE DO MARANHAO; ANAJATUBA; ANAPURUS; APICUM-ACU; ARAGUANA; ARAIOSES; ARAME; ARARI; AXIXA; BACABAL; BACABEIRA; BACURI; BACURITUBA; BALSAS; BARAO DE GRAJAU; BARRA DO CORDA; BARREIRINHAS; BELAGUA; BELA VISTA DO MARANHAO; BENEDITO LEITE; BEQUIMAO; BERNARDO DO MEARIM; BOA VISTA DO GURUPI; BOM JARDIM; BOM JESUS DAS SELVAS; BOM LUGAR; BREJO; BREJO DE AREIA; BURITI; BURITI BRAVO; BURITICUPU; BURITIRANA; CACHOEIRA GRANDE; CAJAPIO; CAJARI; CAMPESTRE DO MARANHAO; CANDIDO MENDES; CANTANHEDE; CAPINZAL DO NORTE; CAROLINA; CARUTAPERA; CAXIAS; CEDRAL; CENTRAL DO MARANHAO; CENTRO DO GUILHERME; CENTRO NOVO DO MARANHAO; CHAPADINHA; CIDELANDIA; CODO; COELHO NETO; COLINAS; CONCEICAO DO LAGO-ACU; COROATA; CURURUPU; DAVINOPOLIS; DOM PEDRO; DUQUE BACELAR; ESPERANTINOPOLIS; ESTREITO; FEIRA NOVA DO MARANHAO; FERNANDO FALCAO; FORMOSA DA SERRA NEGRA; FORTALEZA DOS NOGUEIRAS; FORTUNA; GODOFREDO VIANA; GONCALVES DIAS; GOVERNADOR ARCHER; GOVERNADOR EDISON LOBAO; GOVERNADOR EUGENIO BARROS; GOVERNADOR LUIZ ROCHA; GOVERNADOR NEWTON BELLO; GOVERNADOR NUNES FREIRE; GRACA ARANHA; GRAJAU; GUIMARAES; HUMBERTO DE CAMPOS; ICATU; IGARAPE DO MEIO; IGARAPE GRANDE; IMPERATRIZ; ITAIPAVA DO GRAJAU; ITAPECURU MIRIM; ITINGA DO MARANHAO; JATOBA; JENIPAPO DOS VIEIRAS; JOAO LISBOA; JOSELANDIA; JUNCO DO MARANHAO; LAGO DA PEDRA; LAGO DO JUNCO; LAGO VERDE; LAGOA DO MATO; LAGO DOS RODRIGUES; LAGOA GRANDE DO MARANHAO; LAJEADO NOVO; LIMA CAMPOS; LORETO; LUIS DOMINGUES; MAGALHAES DE ALMEIDA; MARACACUME; MARAJA DO SENA; MARANHAOZINHO; MATA ROMA; MATINHA; MATOES; MATOES DO NORTE; MILAGRES DO MARANHAO; MIRADOR; MIRANDA DO NORTE; MIRINZAL; MONCAO; MONTES ALTOS; MORROS; NINA RODRIGUES; NOVA COLINAS; NOVA IORQUE; NOVA OLINDA DO MARANHAO; OLHO D'AGUA DAS CUNHAS; OLINDA NOVA DO MARANHAO; PACO DO LUMIAR; PALMEIRANDIA; PARAIBANO; PARNARAMA; PASSAGEM FRANCA; PASTOS BONS; PAULINO NEVES; PAULO RAMOS; PEDREIRAS; PEDRO DO ROSARIO; PENALVA; PERI MIRIM; PERITORO; PINDARE-MIRIM; PINHEIRO; PIO XII; PIRAPEMAS; POCAO DE PEDRAS; PORTO FRANCO; PORTO RICO DO MARANHAO; PRESIDENTE DUTRA; PRESIDENTE JUSCELINO; PRESIDENTE MEDICI; PRESIDENTE SARNEY; PRESIDENTE VARGAS; PRIMEIRA CRUZ; RAPOSA; RIACHAO; RIBAMAR FIQUENE; ROSARIO; SAMBAIBA; SANTA FILOMENA DO MARANHAO; SANTA HELENA; SANTA INES; SANTA LUZIA; SANTA LUZIA DO PARUA; SANTA QUITERIA DO MARANHAO; SANTA RITA; SANTANA DO MARANHAO; SANTO AMARO DO MARANHAO; SANTO ANTONIO DOS LOPES; SAO BENEDITO DO RIO PRETO; SAO BENTO; SAO BERNARDO; SAO DOMINGOS DO AZEITAO; SAO DOMINGOS DO MARANHAO; SAO FELIX DE BALSAS; SAO FRANCISCO DO BREJAO; SAO FRANCISCO DO MARANHAO; SAO JOAO BATISTA; SAO JOAO DO CARU; SAO JOAO DO PARAISO; SAO JOAO DO SOTER; SAO JOAO DOS PATOS; SAO JOSE DE RIBAMAR; SAO JOSE DOS BASILIOS; SAO LUIS; SAO LUIS GONZAGA DO MARANHAO; SAO MATEUS DO MARANHAO; SAO PEDRO DA AGUA BRANCA; SAO PEDRO DOS CRENTES; SAO RAIMUNDO DAS MANGABEIRAS; SAO RAIMUNDO DO DOCA BEZERRA; SAO ROBERTO; SAO VICENTE FERRER; SATUBINHA; SENADOR ALEXANDRE COSTA; SENADOR LA ROCQUE; SERRANO DO MARANHAO; SITIO NOVO; SUCUPIRA DO NORTE; SUCUPIRA DO RIACHAO; TASSO FRAGOSO; TIMBIRAS; TIMON; TRIZIDELA DO VALE; TUFILANDIA; TUNTUM; TURIACU; TURILANDIA; TUTOIA; URBANO SANTOS; VARGEM GRANDE; VIANA; VILA NOVA DOS MARTIRIOS; VITORIA DO MEARIM; VITORINO FREIRE; ZE DOCA</t>
-  </si>
-  <si>
-    <t>210005; 210010; 210015; 210020; 210030; 210040; 210043; 210047; 210050; 210055; 210060; 210070; 210080; 210083; 210087; 210090; 210095; 210100; 210110; 210120; 210125; 210130; 210135; 210140; 210150; 210160; 210170; 210173; 210177; 210180; 210190; 210193; 210197; 210200; 210203; 210207; 210210; 210215; 210220; 210230; 210232; 210235; 210237; 210240; 210250; 210255; 210260; 210270; 210275; 210280; 210290; 210300; 210310; 210312; 210315; 210317; 210320; 210325; 210330; 210340; 210350; 210355; 210360; 210370; 210375; 210380; 210390; 210400; 210405; 210407; 210408; 210409; 210410; 210420; 210430; 210440; 210450; 210455; 210460; 210462; 210465; 210467; 210470; 210480; 210490; 210500; 210510; 210515; 210520; 210530; 210535; 210540; 210542; 210545; 210547; 210550; 210560; 210565; 210570; 210580; 210590; 210592; 210594; 210596; 210598; 210600; 210610; 210620; 210630; 210632; 210635; 210637; 210640; 210650; 210660; 210663; 210667; 210670; 210675; 210680; 210690; 210700; 210710; 210720; 210725; 210730; 210735; 210740; 210745; 210750; 210760; 210770; 210780; 210790; 210800; 210805; 210810; 210820; 210825; 210830; 210840; 210845; 210850; 210860; 210870; 210880; 210890; 210900; 210905; 210910; 210920; 210923; 210927; 210930; 210940; 210945; 210950; 210955; 210960; 210970; 210975; 210980; 210990; 211000; 211003; 211010; 211020; 211023; 211027; 211030; 211040; 211050; 211060; 211065; 211070; 211080; 211085; 211090; 211100; 211102; 211105; 211107; 211110; 211120; 211125; 211130; 211140; 211150; 211153; 211157; 211160; 211163; 211167; 211170; 211172; 211174; 211176; 211178; 211180; 211190; 211195; 211200; 211210; 211220; 211223; 211227; 211230; 211240; 211245; 211250; 211260; 211270; 211280; 211285; 211290; 211300; 211400</t>
-  </si>
-  <si>
-    <t>7153262</t>
+    <t>Com o Programa Nacional de Redução das Filas de Cirurgias Eletivas, instituído pela Portaria GM/MS nº 90, de 03 de fevereiro de 2023, o Governo Federal deu um passo fundamental para enfrentar a questão das filas para cirurgias eletivas, exames complementares e consultas especializadas no Sistema Único de Saúde (SUS), incentivando desta forma na organização de mutirões em todo o país, a fim de desafogar a demanda reprimida. A Priore os recursos financeiros disponíveis em 2023 para o Programa Nacional estão previstos a partir de um cálculo baseado na população dos estados, o restante será repassado de acordo com a produção apresentada de cirurgias realizadas. São objetivos do Programa a organização e ampliação do acesso a cirurgias, exames e consultas na Atenção Especializada (em especial, quando forem identificadas demandas reprimidas); o aprimoramento da governança da Rede de Atenção à Saúde; o fomento ao monitoramento e à avaliação das ações e dos serviços de saúde; a qualificação da contratualização com a rede complementar; a mudança do modelo de gestão e regulação das filas para a atenção especializada; e o fomento à implementação de um novo modelo de custeio para a atenção ambulatorial especializada e para a realização de cirurgias eletivas. O Programa prevê estratégias para garantir equipes cirúrgicas completas e melhorar o fluxo de atendimento em todo o Brasil. O Estado do Maranhão estabelecerá as cirurgias prioritárias, de acordo com a realidade de cada município. Em cumprimento ao Programa Nacional de Redução das Filas de Cirurgias Eletivas a Secretaria de Estado da Saúde do Maranhão envidará esforços nas ações para melhoria de processos de gestão das filas e do fluxo</t>
+  </si>
+  <si>
+    <t>0, 0</t>
+  </si>
+  <si>
+    <t>ACAILANDIA; AMARANTE DO MARANHAO; BALSAS; BARRA DO CORDA; BURITI BRAVO; BURITICUPU; CAROLINA; CIDELANDIA; COELHO NETO; COLINAS; CONCEICAO DO LAGO-ACU; IMPERATRIZ; ITAIPAVA DO GRAJAU; JENIPAPO DOS VIEIRAS; LAGO DA PEDRA; LIMA CAMPOS; MATOES; MIRINZAL; PARNARAMA; PINHEIRO; PIRAPEMAS; POCAO DE PEDRAS; PRESIDENTE JUSCELINO; SANTA HELENA; SANTA RITA; SANTANA DO MARANHAO; SAO FRANCISCO DO MARANHAO; SAO JOAO DO SOTER; SAO JOAO DOS PATOS; SAO JOSE DE RIBAMAR; SAO LUIS; SAO PEDRO DOS CRENTES; SATUBINHA; TIMBIRAS; TIMON; TUNTUM</t>
+  </si>
+  <si>
+    <t>210005; 210060; 210140; 210160; 210230; 210232; 210280; 210325; 210340; 210350; 210355; 210530; 210535; 210547; 210570; 210600; 210660; 210680; 210780; 210860; 210880; 210890; 210920; 210980; 211020; 211023; 211090; 211107; 211110; 211120; 211130; 211157; 211172; 211210; 211220; 211230</t>
+  </si>
+  <si>
+    <t>2870060</t>
   </si>
   <si>
     <t>20.120.029,55</t>
@@ -767,9 +828,6 @@
   </si>
   <si>
     <t>Há uma demanda reprimida para procedimentos cirúrgicos eletivos de media e alta complexidade, potencializada pela Pandemia Covid 19. A Secretaria de Estado da Saúde do Maranhão em conjunto com os municípios descentralizou os serviços de saúde ambulatoriais e hospitalares para as 19 Regiões de Saúde, abrangendo os 217 municípios maranhenses. Desta feita, os procedimentos cirúrgicos eletivos serão realizados nos estabelecimentos de saúde de gestão estadual e municipal</t>
-  </si>
-  <si>
-    <t>Não</t>
   </si>
   <si>
     <t>Para ampliação dos serviços será necessário implementar os serviços nos estabelecimentos de saude adotando as seguintes medidas:
@@ -780,6 +838,250 @@
   </si>
   <si>
     <t>A gestão da fila cirúrgica será realizada pela gestão estadual com sistema de compartilhamento com os municípios, visando o acompanhamento das metas programadas e realizadas por cada estabelecimento de saúde e cronograma de execução estabelecido no Plano Nacional de Redução de Filas</t>
+  </si>
+  <si>
+    <t>170553</t>
+  </si>
+  <si>
+    <t>03.517.102/0001-77</t>
+  </si>
+  <si>
+    <t>FUNDO ESPECIAL DE SAUDE</t>
+  </si>
+  <si>
+    <t>A população estimada de Mato Grosso do Sul de 2.839.188 habitantes e a extensão territorial de 357.147,995 km², com densidade demográfica de 6,86 hab/km², de acordo com IBGE, Mato Grosso do Sul | Cidades e Estados | IBGE em 26 de agosto de 2022.
+O desenho regional da saúde é dividido por quatro macrorregiões de saúde, sendo elas Campo Grande, Dourados, Três Lagoas e Corumbá.
+O Estado dispõe de 77 serviços hospitalares, sendo 22 serviços de gestão municipal e 46 de gestão estadual. Os hospitais com maior densidade tecnológica ficam sob gestão municipal e a maioria dos hospitais de pequeno porte sob gestão estadual.</t>
+  </si>
+  <si>
+    <t>ANGELICA CRISTINA SEGATTO CONGRO</t>
+  </si>
+  <si>
+    <t>angelica.congro@saude.ms.gov.br</t>
+  </si>
+  <si>
+    <t>67 33181669; 67 33181669</t>
+  </si>
+  <si>
+    <t>170589</t>
+  </si>
+  <si>
+    <t>03.609.595/0001-75</t>
+  </si>
+  <si>
+    <t>FUNDO ESTADUAL DE SAUDE DO ESTADO DA PARAIBA - FESEP</t>
+  </si>
+  <si>
+    <t>JOAO PESSOA</t>
+  </si>
+  <si>
+    <t>PB</t>
+  </si>
+  <si>
+    <t>Considerando os esforços desta Secretaria de Saúde do Estado em organizar a sua rede de assistência e a missão de fazer saúde com qualidade de eficiência, garantindo acesso a todos os usuários paraibanos, que busquem assistência em Cirurgias Eletivas, Exames Complementares e Consultas Especializadas, visto que a demanda de cirurgias é muito alta, que o recurso financeiro irá ajudar na redução do tempo de espera dos pacientes e desafogar a demanda represada, estamos encaminhando proposta para habilitação no Programa Nacional de Redução das Filas de Cirurgias Eletivas, Exames Complementares e Consultas Especializadas no Sistema Único de Saúde (SUS).</t>
+  </si>
+  <si>
+    <t>AGUA BRANCA; AGUIAR; ALAGOA GRANDE; ALAGOA NOVA; ALAGOINHA; ALCANTIL; ALGODAO DE JANDAIRA; ALHANDRA; SAO JOAO DO RIO DO PEIXE; AMPARO; APARECIDA; ARACAGI; ARARA; ARARUNA; AREIA; AREIA DE BARAUNAS; AREIAL; AROEIRAS; ASSUNCAO; BAIA DA TRAICAO; BANANEIRAS; BARAUNA; BARRA DE SANTANA; BARRA DE SANTA ROSA; BARRA DE SAO MIGUEL; BAYEUX; BELEM; BELEM DO BREJO DO CRUZ; BERNARDINO BATISTA; BOA VENTURA; BOA VISTA; BOM JESUS; BOM SUCESSO; BONITO DE SANTA FE; BOQUEIRAO; IGARACY; BORBOREMA; BREJO DO CRUZ; BREJO DOS SANTOS; CAAPORA; CABACEIRAS; CABEDELO; CACHOEIRA DOS INDIOS; CACIMBA DE AREIA; CACIMBA DE DENTRO; CACIMBAS; CAICARA; CAJAZEIRAS; CAJAZEIRINHAS; CALDAS BRANDAO; CAMALAU; CAMPINA GRANDE; CAPIM; CARAUBAS; CARRAPATEIRA; CASSERENGUE; CATINGUEIRA; CATOLE DO ROCHA; CATURITE; CONCEICAO; CONDADO; CONDE; CONGO; COREMAS; COXIXOLA; CRUZ DO ESPIRITO SANTO; CUBATI; CUITE; CUITEGI; CUITE DE MAMANGUAPE; CURRAL DE CIMA; CURRAL VELHO; DAMIAO; DESTERRO; VISTA SERRANA; DIAMANTE; DONA INES; DUAS ESTRADAS; EMAS; ESPERANCA; FAGUNDES; FREI MARTINHO; GADO BRAVO; GUARABIRA; GURINHEM; GURJAO; IBIARA; IMACULADA; INGA; ITABAIANA; ITAPORANGA; ITAPOROROCA; ITATUBA; JACARAU; JERICO; JOAO PESSOA; JUAREZ TAVORA; JUAZEIRINHO; JUNCO DO SERIDO; JURIPIRANGA; JURU; LAGOA; LAGOA DE DENTRO; LAGOA SECA; LASTRO; LIVRAMENTO; LOGRADOURO; LUCENA; MAE D'AGUA; MALTA; MAMANGUAPE; MANAIRA; MARCACAO; MARI; MARIZOPOLIS; MASSARANDUBA; MATARACA; MATINHAS; MATO GROSSO; MATUREIA; MOGEIRO; MONTADAS; MONTE HOREBE; MONTEIRO; MULUNGU; NATUBA; NAZAREZINHO; NOVA FLORESTA; NOVA OLINDA; NOVA PALMEIRA; OLHO D'AGUA; OLIVEDOS; OURO VELHO; PARARI; PASSAGEM; PATOS; PAULISTA; PEDRA BRANCA; PEDRA LAVRADA; PEDRAS DE FOGO; PIANCO; PICUI; PILAR; PILOES; PILOEZINHOS; PIRPIRITUBA; PITIMBU; POCINHOS; POCO DANTAS; POCO DE JOSE DE MOURA; POMBAL; PRATA; PRINCESA ISABEL; PUXINANA; QUEIMADAS; QUIXABA; REMIGIO; PEDRO REGIS; RIACHAO; RIACHAO DO BACAMARTE; RIACHAO DO POCO; RIACHO DE SANTO ANTONIO; RIACHO DOS CAVALOS; RIO TINTO; SALGADINHO; SALGADO DE SAO FELIX; SANTA CECILIA; SANTA CRUZ; SANTA HELENA; SANTA INES; SANTA LUZIA; SANTANA DE MANGUEIRA; SANTANA DOS GARROTES; JOCA CLAUDINO; SANTA RITA; SANTA TERESINHA; SANTO ANDRE; SAO BENTO; SAO BENTINHO; SAO DOMINGOS DO CARIRI; SAO DOMINGOS; SAO FRANCISCO; SAO JOAO DO CARIRI; SAO JOAO DO TIGRE; SAO JOSE DA LAGOA TAPADA; SAO JOSE DE CAIANA; SAO JOSE DE ESPINHARAS; SAO JOSE DOS RAMOS; SAO JOSE DE PIRANHAS; SAO JOSE DE PRINCESA; SAO JOSE DO BONFIM; SAO JOSE DO BREJO DO CRUZ; SAO JOSE DO SABUGI; SAO JOSE DOS CORDEIROS; SAO MAMEDE; SAO MIGUEL DE TAIPU; SAO SEBASTIAO DE LAGOA DE ROCA; SAO SEBASTIAO DO UMBUZEIRO; SAPE; SAO VICENTE DO SERIDO; SERRA BRANCA; SERRA DA RAIZ; SERRA GRANDE; SERRA REDONDA; SERRARIA; SERTAOZINHO; SOBRADO; SOLANEA; SOLEDADE; SOSSEGO; SOUSA; SUME; TACIMA; TAPEROA; TAVARES; TEIXEIRA; TENORIO; TRIUNFO; UIRAUNA; UMBUZEIRO; VARZEA; VIEIROPOLIS; ZABELE</t>
+  </si>
+  <si>
+    <t>250010; 250020; 250030; 250040; 250050; 250053; 250057; 250060; 250070; 250073; 250077; 250080; 250090; 250100; 250110; 250115; 250120; 250130; 250135; 250140; 250150; 250153; 250157; 250160; 250170; 250180; 250190; 250200; 250205; 250210; 250215; 250220; 250230; 250240; 250250; 250260; 250270; 250280; 250290; 250300; 250310; 250320; 250330; 250340; 250350; 250355; 250360; 250370; 250375; 250380; 250390; 250400; 250403; 250407; 250410; 250415; 250420; 250430; 250435; 250440; 250450; 250460; 250470; 250480; 250485; 250490; 250500; 250510; 250520; 250523; 250527; 250530; 250535; 250540; 250550; 250560; 250570; 250580; 250590; 250600; 250610; 250620; 250625; 250630; 250640; 250650; 250660; 250670; 250680; 250690; 250700; 250710; 250720; 250730; 250740; 250750; 250760; 250770; 250780; 250790; 250800; 250810; 250820; 250830; 250840; 250850; 250855; 250860; 250870; 250880; 250890; 250900; 250905; 250910; 250915; 250920; 250930; 250933; 250937; 250939; 250940; 250950; 250960; 250970; 250980; 250990; 251000; 251010; 251020; 251030; 251040; 251050; 251060; 251065; 251070; 251080; 251090; 251100; 251110; 251120; 251130; 251140; 251150; 251160; 251170; 251180; 251190; 251200; 251203; 251207; 251210; 251220; 251230; 251240; 251250; 251260; 251270; 251272; 251274; 251275; 251276; 251278; 251280; 251290; 251300; 251310; 251315; 251320; 251330; 251335; 251340; 251350; 251360; 251365; 251370; 251380; 251385; 251390; 251392; 251394; 251396; 251398; 251400; 251410; 251420; 251430; 251440; 251445; 251450; 251455; 251460; 251465; 251470; 251480; 251490; 251500; 251510; 251520; 251530; 251540; 251550; 251560; 251570; 251580; 251590; 251593; 251597; 251600; 251610; 251615; 251620; 251630; 251640; 251650; 251660; 251670; 251675; 251680; 251690; 251700; 251710; 251720; 251740</t>
+  </si>
+  <si>
+    <t>4059905</t>
+  </si>
+  <si>
+    <t>LUCIANO PINHEIRO DA NOBREGA JUNIOR</t>
+  </si>
+  <si>
+    <t>pinheiro.lucianojr@gmail.com</t>
+  </si>
+  <si>
+    <t>83 96552274</t>
+  </si>
+  <si>
+    <t>28/02/2023</t>
+  </si>
+  <si>
+    <t>29/05/2023</t>
+  </si>
+  <si>
+    <t>LUCIANO PINHEIRO DA NÓBREGA JÚNIOR</t>
+  </si>
+  <si>
+    <t>CHEFE DE NÚCLEO DE PROCESSAMENTO</t>
+  </si>
+  <si>
+    <t>(83) 99655-2274</t>
+  </si>
+  <si>
+    <t>170595</t>
+  </si>
+  <si>
+    <t>07.458.465/0001-30</t>
+  </si>
+  <si>
+    <t>FUNDO ESTADUAL DE SAUDE - FUNDES</t>
+  </si>
+  <si>
+    <t>RIO BRANCO</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>ACRELANDIA; ASSIS BRASIL; BRASILEIA; BUJARI; CAPIXABA; CRUZEIRO DO SUL; EPITACIOLANDIA; FEIJO; JORDAO; MANCIO LIMA; MANOEL URBANO; MARECHAL THAUMATURGO; PLACIDO DE CASTRO; PORTO WALTER; RIO BRANCO; RODRIGUES ALVES; SANTA ROSA DO PURUS; SENADOR GUIOMARD; SENA MADUREIRA; TARAUACA; XAPURI; PORTO ACRE</t>
+  </si>
+  <si>
+    <t>120001; 120005; 120010; 120013; 120017; 120020; 120025; 120030; 120032; 120033; 120034; 120035; 120038; 120039; 120040; 120042; 120043; 120045; 120050; 120060; 120070; 120080</t>
+  </si>
+  <si>
+    <t>906876</t>
+  </si>
+  <si>
+    <t>MONALISA RAFAELY ZAFFONATO DA ROSA</t>
+  </si>
+  <si>
+    <t>monalisarzr.bio@gmail.com</t>
+  </si>
+  <si>
+    <t>68 99533552</t>
+  </si>
+  <si>
+    <t>170625</t>
+  </si>
+  <si>
+    <t>12.116.247/0001-57</t>
+  </si>
+  <si>
+    <t>FUNDO DE SAUDE DO DISTRITO FEDERAL</t>
+  </si>
+  <si>
+    <t>BRASILIA</t>
+  </si>
+  <si>
+    <t>DF</t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>BRASILIA; REGIAO ADMINISTRATIVA DE AGUAS CLARAS; REGIAO ADMINISTRATIVA DE BRAZLANDIA; REGIAO ADMINISTRATIVA DE CANDANGOLANDIA; REGIAO ADMINISTRATIVA DE CEILANDIA; REGIAO ADMINISTRATIVA DO CRUZEIRO; REGIAO ADMINISTRATIVA DO GAMA; REGIAO ADMINISTRATIVA DO GUARA; REGIAO ADMINISTRATIVA DO LAGO NORTE; REGIAO ADMINISTRATIVA DO LAGO SUL; REGIAO ADMINISTRATIVA DO NUCLEO BANDEIRANTES; REGIAO ADMINISTRATIVA DO PARANOA; REGIAO ADMINISTRATIVA DO PARK WAY; REGIAO ADMINISTRATIVA DE PLANALTINA; REGIAO ADMINISTRATIVA DE RECANTO DA EMAS; REGIAO ADMINISTRATIVA DO RIACHO FUNDO I; REGIAO ADMINISTRATIVA DO RIACHO FUNDO II; REGIAO ADMINISTRATIVA DE SAMAMBAIA; REGIAO ADMINISTRATIVA DE SANTA MARIA; REGIAO ADMINISTRATIVA DE SAO SEBASTIAO; REGIAO ADMINISTRATIVA DE SOBRADINHO; REGIAO ADMINISTRATIVA DE SOBRADINHO II; REGIAO ADMINISTRATIVA DE TAGUATINGA; REGIAO ADMINISTRATIVA DO VARJAO; REGIAO ADMINISTRATIVA DO ITAPOA; REGIAO ADMINISTRATIVA DO JARDIM BOTANICO; REGIAO ADMINISTRATIVA DO SUDOESTE/OCTOGONAL; REGIAO ADMINISTRATIVA DE SCIA (ESTRUTURAL); REGIAO ADMINISTRATIVA DE VICENTE PIRES; REGIAO ADMINISTRATIVA DO SIA; REGIAO ADMINISTRATIVA DA FERCAL; REGIAO ADMINISTRATIVA DA ARNIQUEIRAS; REGIAO ADMINISTRATIVA DA ASA NORTE; REGIAO ADMINISTRATIVA DA ASA SUL</t>
+  </si>
+  <si>
+    <t>530010; 539901; 539902; 539903; 539904; 539905; 539906; 539907; 539908; 539909; 539910; 539912; 539913; 539914; 539915; 539916; 539917; 539918; 539919; 539920; 539921; 539922; 539924; 539925; 539928; 539930; 539931; 539933; 539934; 539935; 539936; 539938; 539939; 539940</t>
+  </si>
+  <si>
+    <t>3094325</t>
+  </si>
+  <si>
+    <t>8.703.429,35</t>
+  </si>
+  <si>
+    <t>LUDMILA DE ORNELLAS ABREU</t>
+  </si>
+  <si>
+    <t>gcch.sesdf@gmail.com</t>
+  </si>
+  <si>
+    <t>61 81159681</t>
+  </si>
+  <si>
+    <t>01/03/2023</t>
+  </si>
+  <si>
+    <t>30/05/2023</t>
+  </si>
+  <si>
+    <t>170640</t>
+  </si>
+  <si>
+    <t>06.206.659/0001-85</t>
+  </si>
+  <si>
+    <t>FUNDO DE SAUDE DO ESTADO DO PIAUI</t>
+  </si>
+  <si>
+    <t>TERESINA</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>CONSIDERANDO Portaria GM/MS nº 90, de 3 de fevereiro de 2023 que Institui o Programa Nacional de Redução das Filas de Cirurgias Eletivas, Exames Complementares e Consultas Especializadas com destinação de R$ 600.000,00 para os 27 Estados Federados e especificamente R$ 9.251.808,75 ao estado do Piauí.
+Com base nos aspectos normativos do Ministério da Saúde, na existência de fila de espera por cirurgias eletivas, na disponibilidade de recursos financeiros e na capacidade instalada para a realização das cirurgias nas Unidades Hospitalares de Gerenciamento Estadual, Municipal e serviços contratualizados e na garantia de seguimento do tratamento pós-cirúrgicos, a SESAPI/SUGMAC/DUDOH apresenta o Plano DE TRABALHO PARA REDUÇÃO DAS FILAS DE CIRURGIAS ELETIVAS NO ESTADO DO PIAUÍ- 2023, visando a melhoria do acesso de forma regulada e com pactuação junto aos Municípios do estado do Piauí, através da Comissão Intergestores Bipartite (CIB).</t>
+  </si>
+  <si>
+    <t>Enviada para o MS</t>
+  </si>
+  <si>
+    <t>ACAUA; AGRICOLANDIA; AGUA BRANCA; ALAGOINHA DO PIAUI; ALEGRETE DO PIAUI; ALTO LONGA; ALTOS; ALVORADA DO GURGUEIA; AMARANTE; ANGICAL DO PIAUI; ANISIO DE ABREU; ANTONIO ALMEIDA; AROAZES; AROEIRAS DO ITAIM; ARRAIAL; ASSUNCAO DO PIAUI; AVELINO LOPES; BAIXA GRANDE DO RIBEIRO; BARRA D'ALCANTARA; BARRAS; BARREIRAS DO PIAUI; BARRO DURO; BATALHA; BELA VISTA DO PIAUI; BELEM DO PIAUI; BENEDITINOS; BERTOLINIA; BETANIA DO PIAUI; BOA HORA; BOCAINA; BOM JESUS; BOM PRINCIPIO DO PIAUI; BONFIM DO PIAUI; BOQUEIRAO DO PIAUI; BRASILEIRA; BREJO DO PIAUI; BURITI DOS LOPES; BURITI DOS MONTES; CABECEIRAS DO PIAUI; CAJAZEIRAS DO PIAUI; CAJUEIRO DA PRAIA; CALDEIRAO GRANDE DO PIAUI; CAMPINAS DO PIAUI; CAMPO ALEGRE DO FIDALGO; CAMPO GRANDE DO PIAUI; CAMPO LARGO DO PIAUI; CAMPO MAIOR; CANAVIEIRA; CANTO DO BURITI; CAPITAO DE CAMPOS; CAPITAO GERVASIO OLIVEIRA; CARACOL; CARAUBAS DO PIAUI; CARIDADE DO PIAUI; CASTELO DO PIAUI; CAXINGO; COCAL; COCAL DE TELHA; COCAL DOS ALVES; COIVARAS; COLONIA DO GURGUEIA; COLONIA DO PIAUI; CONCEICAO DO CANINDE; CORONEL JOSE DIAS; CORRENTE; CRISTALANDIA DO PIAUI; CRISTINO CASTRO; CURIMATA; CURRAIS; CURRALINHOS; CURRAL NOVO DO PIAUI; DEMERVAL LOBAO; DIRCEU ARCOVERDE; DOM EXPEDITO LOPES; DOMINGOS MOURAO; DOM INOCENCIO; ELESBAO VELOSO; ELISEU MARTINS; ESPERANTINA; FARTURA DO PIAUI; FLORES DO PIAUI; FLORESTA DO PIAUI; FLORIANO; FRANCINOPOLIS; FRANCISCO AYRES; FRANCISCO MACEDO; FRANCISCO SANTOS; FRONTEIRAS; GEMINIANO; GILBUES; GUADALUPE; GUARIBAS; HUGO NAPOLEAO; ILHA GRANDE; INHUMA; IPIRANGA DO PIAUI; ISAIAS COELHO; ITAINOPOLIS; ITAUEIRA; JACOBINA DO PIAUI; JAICOS; JARDIM DO MULATO; JATOBA DO PIAUI; JERUMENHA; JOAO COSTA; JOAQUIM PIRES; JOCA MARQUES; JOSE DE FREITAS; JUAZEIRO DO PIAUI; JULIO BORGES; JUREMA; LAGOINHA DO PIAUI; LAGOA ALEGRE; LAGOA DO BARRO DO PIAUI; LAGOA DE SAO FRANCISCO; LAGOA DO PIAUI; LAGOA DO SITIO; LANDRI SALES; LUIS CORREIA; LUZILANDIA; MADEIRO; MANOEL EMIDIO; MARCOLANDIA; MARCOS PARENTE; MASSAPE DO PIAUI; MATIAS OLIMPIO; MIGUEL ALVES; MIGUEL LEAO; MILTON BRANDAO; MONSENHOR GIL; MONSENHOR HIPOLITO; MONTE ALEGRE DO PIAUI; MORRO CABECA NO TEMPO; MORRO DO CHAPEU DO PIAUI; MURICI DOS PORTELAS; NAZARE DO PIAUI; NAZARIA; NOSSA SENHORA DE NAZARE; NOSSA SENHORA DOS REMEDIOS; NOVO ORIENTE DO PIAUI; NOVO SANTO ANTONIO; OEIRAS; OLHO D'AGUA DO PIAUI; PADRE MARCOS; PAES LANDIM; PAJEU DO PIAUI; PALMEIRA DO PIAUI; PALMEIRAIS; PAQUETA; PARNAGUA; PARNAIBA; PASSAGEM FRANCA DO PIAUI; PATOS DO PIAUI; PAU D'ARCO DO PIAUI; PAULISTANA; PAVUSSU; PEDRO II; PEDRO LAURENTINO; NOVA SANTA RITA; PICOS; PIMENTEIRAS; PIO IX; PIRACURUCA; PIRIPIRI; PORTO; PORTO ALEGRE DO PIAUI; PRATA DO PIAUI; QUEIMADA NOVA; REDENCAO DO GURGUEIA; REGENERACAO; RIACHO FRIO; RIBEIRA DO PIAUI; RIBEIRO GONCALVES; RIO GRANDE DO PIAUI; SANTA CRUZ DO PIAUI; SANTA CRUZ DOS MILAGRES; SANTA FILOMENA; SANTA LUZ; SANTANA DO PIAUI; SANTA ROSA DO PIAUI; SANTO ANTONIO DE LISBOA; SANTO ANTONIO DOS MILAGRES; SANTO INACIO DO PIAUI; SAO BRAZ DO PIAUI; SAO FELIX DO PIAUI; SAO FRANCISCO DE ASSIS DO PIAUI; SAO FRANCISCO DO PIAUI; SAO GONCALO DO GURGUEIA; SAO GONCALO DO PIAUI; SAO JOAO DA CANABRAVA; SAO JOAO DA FRONTEIRA; SAO JOAO DA SERRA; SAO JOAO DA VARJOTA; SAO JOAO DO ARRAIAL; SAO JOAO DO PIAUI; SAO JOSE DO DIVINO; SAO JOSE DO PEIXE; SAO JOSE DO PIAUI; SAO JULIAO; SAO LOURENCO DO PIAUI; SAO LUIS DO PIAUI; SAO MIGUEL DA BAIXA GRANDE; SAO MIGUEL DO FIDALGO; SAO MIGUEL DO TAPUIO; SAO PEDRO DO PIAUI; SAO RAIMUNDO NONATO; SEBASTIAO BARROS; SEBASTIAO LEAL; SIGEFREDO PACHECO; SIMOES; SIMPLICIO MENDES; SOCORRO DO PIAUI; SUSSUAPARA; TAMBORIL DO PIAUI; TANQUE DO PIAUI; TERESINA; UNIAO; URUCUI; VALENCA DO PIAUI; VARZEA BRANCA; VARZEA GRANDE; VERA MENDES; VILA NOVA DO PIAUI; WALL FERRAZ</t>
+  </si>
+  <si>
+    <t>220005; 220010; 220020; 220025; 220027; 220030; 220040; 220045; 220050; 220060; 220070; 220080; 220090; 220095; 220100; 220105; 220110; 220115; 220117; 220120; 220130; 220140; 220150; 220155; 220157; 220160; 220170; 220173; 220177; 220180; 220190; 220191; 220192; 220194; 220196; 220198; 220200; 220202; 220205; 220207; 220208; 220209; 220210; 220211; 220213; 220217; 220220; 220225; 220230; 220240; 220245; 220250; 220253; 220255; 220260; 220265; 220270; 220271; 220272; 220273; 220275; 220277; 220280; 220285; 220290; 220300; 220310; 220320; 220323; 220325; 220327; 220330; 220335; 220340; 220342; 220345; 220350; 220360; 220370; 220375; 220380; 220385; 220390; 220400; 220410; 220415; 220420; 220430; 220435; 220440; 220450; 220455; 220460; 220465; 220470; 220480; 220490; 220500; 220510; 220515; 220520; 220525; 220527; 220530; 220535; 220540; 220545; 220550; 220551; 220552; 220553; 220554; 220555; 220556; 220557; 220558; 220559; 220560; 220570; 220580; 220585; 220590; 220595; 220600; 220605; 220610; 220620; 220630; 220635; 220640; 220650; 220660; 220665; 220667; 220669; 220670; 220672; 220675; 220680; 220690; 220695; 220700; 220710; 220720; 220730; 220735; 220740; 220750; 220755; 220760; 220770; 220775; 220777; 220779; 220780; 220785; 220790; 220793; 220795; 220800; 220810; 220820; 220830; 220840; 220850; 220855; 220860; 220865; 220870; 220880; 220885; 220887; 220890; 220900; 220910; 220915; 220920; 220930; 220935; 220937; 220940; 220945; 220950; 220955; 220960; 220965; 220970; 220975; 220980; 220985; 220987; 220990; 220995; 220997; 221000; 221005; 221010; 221020; 221030; 221035; 221037; 221038; 221039; 221040; 221050; 221060; 221062; 221063; 221065; 221070; 221080; 221090; 221093; 221095; 221097; 221100; 221110; 221120; 221130; 221135; 221140; 221150; 221160; 221170</t>
+  </si>
+  <si>
+    <t>3289290</t>
+  </si>
+  <si>
+    <t>9.251.808,75</t>
+  </si>
+  <si>
+    <t>VANDERILO SOARES DE ANCHIETA FILHO</t>
+  </si>
+  <si>
+    <t>vanderilo.soares@saude.pi.gov.br</t>
+  </si>
+  <si>
+    <t>86 94143842</t>
+  </si>
+  <si>
+    <t>01/03/2023 14:31:35</t>
+  </si>
+  <si>
+    <t>JOÃO VICTOR DA SILVA BARBOZA</t>
+  </si>
+  <si>
+    <t>COORDENADOR DE APOIO E ACOMPANHAMENTO AOS MUNICÍPIOS</t>
+  </si>
+  <si>
+    <t>86994991774</t>
+  </si>
+  <si>
+    <t>joao.victor@saude.pi.gov.br // ducara@saude.pi.gov.br</t>
+  </si>
+  <si>
+    <t>CamScanner 03-01-2023 13.28.pdf</t>
+  </si>
+  <si>
+    <t>008/2023</t>
+  </si>
+  <si>
+    <t>Com base em dados fornecidos pelo Complexo Regulador Estadual do Piauí (CRE) referente à fila única da regulação estadual, sistema Hydra, observou-se em 16/02/2022 o total de 15.552 solicitações de procedimento cirúrgico eletivo com tempo médio de espera de 464 dias e tempo mediano de espera de 267 dias. Essa variação se dias se deve ao fato de alguns usuários possivelmente não terem sido retirados do sistema de regulação estadual mesmo tendo realizado a cirurgia eletiva. Isso gera um aumento do desvio padrão que consequentemente aumenta o tempo espera total gerando essa distorção entre o tempo de espera médio e mediano.
+Conforme TABELA 01 - FILA DE PACIENTES PARA PROCEDIMENTO CIRURGICO ELETIVO POR ESTABELECIMENTO SOLICITANTE NO SISTEMA DE REGULAÇÃO ESTADUAL - HYDRA - EM 16/02/2023 observa-se que os estabelecimentos de saúde com maior quantidade de solicitações em espera no sistema: 29,8% Hospital Getúlio Vargas ¿ HGV (4.623); 12,1% Hospital Universitário ¿ HU (1.883); 10,8% Hospital da Polícia Militar ¿ HPM (1.685); 8,7% Hospital Infantil Lucídio Portella ¿ HILP (1.354); 5,2 % Hospital Regional Tibério Nunes (807) e 5,1% Hospital Regional De Campo Maior (793).
+Observa-se que as especialidades médicas com maiores quantidades de solicitações em espera no sistema: 28,37 % Cirurgia Geral (4.407); 16,4% Ortopedia (2.548); 12,47% Ginecologia (1.937) e 11,4% Pediatria Cirúrgica (1.770). 
+Conforme GRÁFICO 02 - FILA DE PACIENTES PARA PROCEDIMENTO CIRURGICO ELETIVO POR MACRORREGIÃO DE SAÚDE NO SISTEMA DE REGULAÇÃO ESTADUAL - HYDRA - EM 16/02/2023 observa-se as macrorregiões de saúde com maior quantidade de solicitações em espera no sistema: 51,9 % Macro Meio Norte (8.058); 18,2% Macro Litoral (2.834); 17,4% Macro Cerrado (2.699); 12,3% Macro Semi Árido (1.906) e 0,2% outras (35) referente a usuários de outros estados cadastrados.
+Conforme GRÁFICO 03 - FILA DE PACIENTES PARA PROCEDIMENTO CIRURGICO ELETIVO POR REGIÃO DE SAÚDE NO SISTEMA DE REGULAÇÃO ESTADUAL - HYDRA - EM 16/02/2023 observa-se nas regiões de saúde com maior quantidade de solicitações em espera no sistema: 43,4% Entre Rios (6.739); 13,8 Cocais (2.147); 8,5% Carnaubais (1.319); 7,5% Vale dos Rios Piauí e Itaueira (1.165) e 6,3% Chapada das Mangabeiras (978).
+Analisada a fila em 16/02/2023 por Procedimento Cirúrgico considerando os códigos tabelados e padronizados pelo Ministério da Saúde observou-se um total de mais de 650 procedimentos eletivos na fila da regulação estadual. Para melhor análise e gestão desses dados, foi elaborada a TABELA 02 com o compilado dos 50 procedimentos com maior quantidade de percentual de usuários em fila. Nesse total de 50 principais procedimentos estão um total de 11.230 solicitações de procedimento correspondendo a um percentual de 72% de toda a fila de cirurgias eletivas no Piauí. Os demais procedimentos além dos 50 principais reúnem mais de 600 códigos de procedimentos foram então somados e totalizaram 4.302 solicitações correspondendo a 27,7% da fila.</t>
+  </si>
+  <si>
+    <t>NAO</t>
+  </si>
+  <si>
+    <t>Organizar e Ampliar o acesso a cirurgias eletivas, em especial àqueles com demanda reprimida identificada através da Fila de Regulação do Acesso a Procedimentos Cirúrgicos Eletivos com execução por Hospitais Públicos e Contratualizados do Piauí em 2023.
+Analisada a fila por Procedimento Cirúrgico considerando os códigos tabelados e padronizados pelo Ministério da Saúde observou-se um total de mais de 650 procedimentos eletivos na fila da regulação estadual. Para melhor análise e gestão desses dados, foi elaborada a TABELA 02 com o compilado dos 50 procedimentos com maior quantidade de percentual de usuários em fila. Nesse total de 50 principais procedimentos estão um total de 11.230 solicitações de procedimento correspondendo a um percentual de 72% de toda a fila de cirurgias eletivas no Piauí. Os demais procedimentos além dos 50 principais reúnem mais de 600 códigos de procedimentos foram então somados e totalizaram 4.302 solicitações correspondendo a 27,7% da fila.
+Analisada a fila o Estado do Piauí juntamente com os Municípios Gestores Plenos vai otimizar a fila de espera para cirurgia eletiva com a inclusão de EAS Públicos Gerenciados pelos municípios e também rede contratualizada. Dessa forma otimiza-se a realização de cirurgias eletivas, qualificação e estímulo a contratualização.</t>
+  </si>
+  <si>
+    <t>Atualmente o a fila de cirurgias eletivas consta no Sistema de Regulação Estadual - HYDRA. Porém, nesse sistema estão inclusos todos as unidades hospitalares de Gerenciamento Estadual, alguns municipais, federal e alguns contratualizados. Porém, com esse estímulo do Plano Nacional de Redução de Filas de Cirurgias Eletivas poderá ser incluídos mais Unidades Hospitais Municipais e Contratualizados que ainda não estão alimentando a fila de cirurgia do Hydra mas que possuem pacientes em fila e realizam procedimento cirúrgico eletivo.</t>
+  </si>
+  <si>
+    <t>plano-atendimento-perf-cir-eletiva-vrs-4a 01.03.2023.xls</t>
+  </si>
+  <si>
+    <t>plano-monitoramento-perf-cir-eletiva-vrs-3-101.03.2023.xls</t>
   </si>
 </sst>
 </file>
@@ -1153,10 +1455,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BY13"/>
+  <dimension ref="A1:BY19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="BY13" sqref="BY13"/>
+      <selection activeCell="BY19" sqref="BY19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2560,7 +2862,7 @@
         <v>79</v>
       </c>
       <c r="AZ6" s="2" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
       <c r="BA6" s="2" t="s">
         <v>79</v>
@@ -2587,31 +2889,31 @@
         <v>79</v>
       </c>
       <c r="BI6" s="2" t="s">
-        <v>79</v>
+        <v>145</v>
       </c>
       <c r="BJ6" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BK6" s="2" t="s">
-        <v>79</v>
+        <v>146</v>
       </c>
       <c r="BL6" s="2" t="s">
-        <v>79</v>
+        <v>146</v>
       </c>
       <c r="BM6" s="2" t="s">
-        <v>79</v>
+        <v>145</v>
       </c>
       <c r="BN6" s="2" t="s">
-        <v>79</v>
+        <v>145</v>
       </c>
       <c r="BO6" s="2" t="s">
         <v>145</v>
       </c>
       <c r="BP6" s="2" t="s">
-        <v>79</v>
+        <v>145</v>
       </c>
       <c r="BQ6" s="2" t="s">
-        <v>79</v>
+        <v>145</v>
       </c>
       <c r="BR6" s="2" t="s">
         <v>145</v>
@@ -2640,7 +2942,7 @@
     </row>
     <row r="7" spans="1:77">
       <c r="A7" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>76</v>
@@ -2661,19 +2963,19 @@
         <v>81</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>87</v>
@@ -2694,13 +2996,13 @@
         <v>79</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="V7" s="2" t="s">
         <v>79</v>
@@ -2769,13 +3071,13 @@
         <v>79</v>
       </c>
       <c r="AR7" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AS7" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AT7" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AU7" s="2" t="s">
         <v>131</v>
@@ -2793,25 +3095,25 @@
         <v>79</v>
       </c>
       <c r="AZ7" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="BA7" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="BB7" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="BC7" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="BD7" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="BE7" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BF7" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="BG7" s="2" t="s">
         <v>79</v>
@@ -2873,7 +3175,7 @@
     </row>
     <row r="8" spans="1:77">
       <c r="A8" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>76</v>
@@ -2894,19 +3196,19 @@
         <v>81</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>123</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>87</v>
@@ -2927,13 +3229,13 @@
         <v>79</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="V8" s="2" t="s">
         <v>79</v>
@@ -3002,19 +3304,19 @@
         <v>79</v>
       </c>
       <c r="AR8" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AS8" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AT8" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AU8" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AV8" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AW8" s="2" t="s">
         <v>79</v>
@@ -3106,7 +3408,7 @@
     </row>
     <row r="9" spans="1:77">
       <c r="A9" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>76</v>
@@ -3127,19 +3429,19 @@
         <v>81</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>87</v>
@@ -3160,13 +3462,13 @@
         <v>79</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="V9" s="2" t="s">
         <v>79</v>
@@ -3235,19 +3537,19 @@
         <v>79</v>
       </c>
       <c r="AR9" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AS9" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AT9" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AU9" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AV9" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AW9" s="2" t="s">
         <v>79</v>
@@ -3339,7 +3641,7 @@
     </row>
     <row r="10" spans="1:77">
       <c r="A10" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>76</v>
@@ -3360,10 +3662,10 @@
         <v>81</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>190</v>
@@ -3492,19 +3794,19 @@
         <v>79</v>
       </c>
       <c r="AZ10" s="2" t="s">
-        <v>79</v>
+        <v>191</v>
       </c>
       <c r="BA10" s="2" t="s">
-        <v>79</v>
+        <v>201</v>
       </c>
       <c r="BB10" s="2" t="s">
-        <v>79</v>
+        <v>202</v>
       </c>
       <c r="BC10" s="2" t="s">
-        <v>79</v>
+        <v>203</v>
       </c>
       <c r="BD10" s="2" t="s">
-        <v>79</v>
+        <v>197</v>
       </c>
       <c r="BE10" s="2" t="s">
         <v>79</v>
@@ -3572,7 +3874,7 @@
     </row>
     <row r="11" spans="1:77">
       <c r="A11" s="2" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>76</v>
@@ -3593,19 +3895,19 @@
         <v>81</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>87</v>
@@ -3626,13 +3928,13 @@
         <v>79</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="V11" s="2" t="s">
         <v>79</v>
@@ -3701,13 +4003,13 @@
         <v>79</v>
       </c>
       <c r="AR11" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="AS11" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="AT11" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="AU11" s="2" t="s">
         <v>199</v>
@@ -3725,19 +4027,19 @@
         <v>79</v>
       </c>
       <c r="AZ11" s="2" t="s">
-        <v>205</v>
+        <v>79</v>
       </c>
       <c r="BA11" s="2" t="s">
-        <v>213</v>
+        <v>79</v>
       </c>
       <c r="BB11" s="2" t="s">
-        <v>214</v>
+        <v>79</v>
       </c>
       <c r="BC11" s="2" t="s">
-        <v>215</v>
+        <v>79</v>
       </c>
       <c r="BD11" s="2" t="s">
-        <v>216</v>
+        <v>79</v>
       </c>
       <c r="BE11" s="2" t="s">
         <v>79</v>
@@ -3805,7 +4107,7 @@
     </row>
     <row r="12" spans="1:77">
       <c r="A12" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>76</v>
@@ -3826,10 +4128,10 @@
         <v>81</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>219</v>
@@ -3892,55 +4194,55 @@
         <v>79</v>
       </c>
       <c r="AD12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR12" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="AE12" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="AF12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AH12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AJ12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AM12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AO12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AP12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AQ12" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR12" s="2" t="s">
+      <c r="AS12" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="AS12" s="2" t="s">
+      <c r="AT12" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="AT12" s="2" t="s">
-        <v>228</v>
       </c>
       <c r="AU12" s="2" t="s">
         <v>199</v>
@@ -3958,19 +4260,19 @@
         <v>79</v>
       </c>
       <c r="AZ12" s="2" t="s">
-        <v>79</v>
+        <v>220</v>
       </c>
       <c r="BA12" s="2" t="s">
-        <v>79</v>
+        <v>228</v>
       </c>
       <c r="BB12" s="2" t="s">
-        <v>79</v>
+        <v>229</v>
       </c>
       <c r="BC12" s="2" t="s">
-        <v>79</v>
+        <v>230</v>
       </c>
       <c r="BD12" s="2" t="s">
-        <v>79</v>
+        <v>231</v>
       </c>
       <c r="BE12" s="2" t="s">
         <v>79</v>
@@ -4038,7 +4340,7 @@
     </row>
     <row r="13" spans="1:77">
       <c r="A13" s="2" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>76</v>
@@ -4059,19 +4361,19 @@
         <v>81</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>231</v>
+        <v>176</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>79</v>
+        <v>236</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>87</v>
@@ -4092,13 +4394,13 @@
         <v>79</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="V13" s="2" t="s">
         <v>79</v>
@@ -4125,10 +4427,10 @@
         <v>79</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="AE13" s="2" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="AF13" s="2" t="s">
         <v>79</v>
@@ -4167,19 +4469,19 @@
         <v>79</v>
       </c>
       <c r="AR13" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="AS13" s="2" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="AT13" s="2" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="AU13" s="2" t="s">
-        <v>241</v>
+        <v>199</v>
       </c>
       <c r="AV13" s="2" t="s">
-        <v>242</v>
+        <v>200</v>
       </c>
       <c r="AW13" s="2" t="s">
         <v>79</v>
@@ -4191,82 +4493,1480 @@
         <v>79</v>
       </c>
       <c r="AZ13" s="2" t="s">
-        <v>233</v>
+        <v>79</v>
       </c>
       <c r="BA13" s="2" t="s">
-        <v>243</v>
+        <v>79</v>
       </c>
       <c r="BB13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BC13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BD13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BE13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BF13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BH13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BK13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BL13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BN13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BP13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BQ13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BR13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BS13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BT13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BU13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BV13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BW13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BX13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BY13" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:77">
+      <c r="A14" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="BC13" s="2" t="s">
+      <c r="B14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="BD13" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="BE13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BF13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BG13" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="BH13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BI13" s="2" t="s">
+      <c r="K14" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD14" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="AE14" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="AF14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR14" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="AS14" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AT14" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="AU14" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="AV14" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="AW14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ14" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="BA14" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="BB14" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="BC14" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="BD14" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="BE14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BF14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG14" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="BH14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI14" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="BJ13" s="2" t="s">
+      <c r="BJ14" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="BK13" s="2" t="s">
+      <c r="BK14" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="BL13" s="2" t="s">
+      <c r="BL14" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="BM13" s="2" t="s">
+      <c r="BM14" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="BN13" s="2" t="s">
+      <c r="BN14" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="BO13" s="2" t="s">
+      <c r="BO14" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="BP13" s="2" t="s">
+      <c r="BP14" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="BQ13" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="BR13" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="BS13" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="BT13" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="BU13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BV13" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="BW13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BX13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BY13" s="2" t="s">
-        <v>79</v>
+      <c r="BQ14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BR14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BS14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BT14" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="BU14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BV14" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="BW14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BX14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BY14" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:77">
+      <c r="A15" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR15" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="AS15" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="AT15" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="AU15" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="AV15" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="AW15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BB15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BC15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BD15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BE15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BF15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BH15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BK15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BL15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BN15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BP15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BQ15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BR15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BS15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BT15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BU15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BV15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BW15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BX15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BY15" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:77">
+      <c r="A16" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="V16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR16" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="AS16" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="AT16" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="AU16" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="AV16" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="AW16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ16" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="BA16" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="BB16" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="BC16" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="BD16" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="BE16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BF16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BH16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BK16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BL16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BN16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BP16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BQ16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BR16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BS16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BT16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BU16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BV16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BW16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BX16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BY16" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:77">
+      <c r="A17" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR17" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="AS17" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="AT17" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="AU17" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="AV17" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="AW17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BB17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BC17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BD17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BE17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BF17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BH17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BK17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BL17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BN17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BP17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BQ17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BR17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BS17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BT17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BU17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BV17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BW17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BX17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BY17" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:77">
+      <c r="A18" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD18" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="AE18" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="AF18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR18" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="AS18" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="AT18" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="AU18" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="AV18" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="AW18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BB18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BC18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BD18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BE18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BF18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BH18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BK18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BL18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BM18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BN18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BP18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BQ18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BR18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BS18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BT18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BU18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BV18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BW18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BX18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BY18" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:77">
+      <c r="A19" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="U19" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD19" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="AE19" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="AF19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR19" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="AS19" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="AT19" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="AU19" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="AV19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW19" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="AX19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ19" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="BA19" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="BB19" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="BC19" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="BD19" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="BE19" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="BF19" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="BG19" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="BH19" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="BI19" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BJ19" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BK19" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BL19" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BM19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BN19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BO19" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BP19" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BQ19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BR19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BS19" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BT19" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="BU19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BV19" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BW19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BX19" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="BY19" s="2" t="s">
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vários ajustes a pedido
</commit_message>
<xml_diff>
--- a/dados/propostas_mon/relatorio_propostas.xlsx
+++ b/dados/propostas_mon/relatorio_propostas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="597">
   <si>
     <t>Nº da Proposta</t>
   </si>
@@ -605,45 +605,6 @@
     <t>dddd</t>
   </si>
   <si>
-    <t>170463</t>
-  </si>
-  <si>
-    <t>11.228.564/0001-00</t>
-  </si>
-  <si>
-    <t>CAMPO GRANDE</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t>XXXX S I M U L A Ç Ã O XXXXXXX</t>
-  </si>
-  <si>
-    <t>AGUA CLARA; ALCINOPOLIS; AMAMBAI; ANASTACIO; ANAURILANDIA; ANGELICA; ANTONIO JOAO; APARECIDA DO TABOADO; AQUIDAUANA; ARAL MOREIRA; BANDEIRANTES; BATAGUASSU; BATAYPORA; BELA VISTA; BODOQUENA; BONITO; BRASILANDIA; CAARAPO; CAMAPUA; CAMPO GRANDE; CARACOL; CASSILANDIA; CHAPADAO DO SUL; CORGUINHO; CORONEL SAPUCAIA; CORUMBA; COSTA RICA; COXIM; DEODAPOLIS; DOIS IRMAOS DO BURITI; DOURADINA; DOURADOS; ELDORADO; FATIMA DO SUL; FIGUEIRAO; GLORIA DE DOURADOS; GUIA LOPES DA LAGUNA; IGUATEMI; INOCENCIA; ITAPORA; ITAQUIRAI; IVINHEMA; JAPORA; JARAGUARI; JARDIM; JATEI; JUTI; LADARIO; LAGUNA CARAPA; MARACAJU; MIRANDA; MUNDO NOVO; NAVIRAI; NIOAQUE; NOVA ALVORADA DO SUL; NOVA ANDRADINA; NOVO HORIZONTE DO SUL; PARAISO DAS AGUAS; PARANAIBA; PARANHOS; PEDRO GOMES; PONTA PORA; PORTO MURTINHO; RIBAS DO RIO PARDO; RIO BRILHANTE; RIO NEGRO; RIO VERDE DE MATO GROSSO; ROCHEDO; SANTA RITA DO PARDO; SAO GABRIEL DO OESTE; SETE QUEDAS; SELVIRIA; SIDROLANDIA; SONORA; TACURU; TAQUARUSSU; TERENOS; TRES LAGOAS; VICENTINA</t>
-  </si>
-  <si>
-    <t>500020; 500025; 500060; 500070; 500080; 500085; 500090; 500100; 500110; 500124; 500150; 500190; 500200; 500210; 500215; 500220; 500230; 500240; 500260; 500270; 500280; 500290; 500295; 500310; 500315; 500320; 500325; 500330; 500345; 500348; 500350; 500370; 500375; 500380; 500390; 500400; 500410; 500430; 500440; 500450; 500460; 500470; 500480; 500490; 500500; 500510; 500515; 500520; 500525; 500540; 500560; 500568; 500570; 500580; 500600; 500620; 500625; 500627; 500630; 500635; 500640; 500660; 500690; 500710; 500720; 500730; 500740; 500750; 500755; 500769; 500770; 500780; 500790; 500793; 500795; 500797; 500800; 500830; 500840</t>
-  </si>
-  <si>
-    <t>2839188</t>
-  </si>
-  <si>
-    <t>MARTA DE SOUSA PANIAGO LEIRIA</t>
-  </si>
-  <si>
-    <t>martapleiria@gmail.com</t>
-  </si>
-  <si>
-    <t>67 99026802</t>
-  </si>
-  <si>
-    <t>22/02/2023</t>
-  </si>
-  <si>
-    <t>23/05/2023</t>
-  </si>
-  <si>
     <t>170490</t>
   </si>
   <si>
@@ -977,9 +938,24 @@
     <t>FUNDO ESPECIAL DE SAUDE</t>
   </si>
   <si>
+    <t>CAMPO GRANDE</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
     <t>A população estimada de Mato Grosso do Sul de 2.839.188 habitantes e a extensão territorial de 357.147,995 km², com densidade demográfica de 6,86 hab/km², de acordo com IBGE, Mato Grosso do Sul | Cidades e Estados | IBGE em 26 de agosto de 2022.
 O desenho regional da saúde é dividido por quatro macrorregiões de saúde, sendo elas Campo Grande, Dourados, Três Lagoas e Corumbá.
 O Estado dispõe de 77 serviços hospitalares, sendo 22 serviços de gestão municipal e 46 de gestão estadual. Os hospitais com maior densidade tecnológica ficam sob gestão municipal e a maioria dos hospitais de pequeno porte sob gestão estadual.</t>
+  </si>
+  <si>
+    <t>AGUA CLARA; ALCINOPOLIS; AMAMBAI; ANASTACIO; ANAURILANDIA; ANGELICA; ANTONIO JOAO; APARECIDA DO TABOADO; AQUIDAUANA; ARAL MOREIRA; BANDEIRANTES; BATAGUASSU; BATAYPORA; BELA VISTA; BODOQUENA; BONITO; BRASILANDIA; CAARAPO; CAMAPUA; CAMPO GRANDE; CARACOL; CASSILANDIA; CHAPADAO DO SUL; CORGUINHO; CORONEL SAPUCAIA; CORUMBA; COSTA RICA; COXIM; DEODAPOLIS; DOIS IRMAOS DO BURITI; DOURADINA; DOURADOS; ELDORADO; FATIMA DO SUL; FIGUEIRAO; GLORIA DE DOURADOS; GUIA LOPES DA LAGUNA; IGUATEMI; INOCENCIA; ITAPORA; ITAQUIRAI; IVINHEMA; JAPORA; JARAGUARI; JARDIM; JATEI; JUTI; LADARIO; LAGUNA CARAPA; MARACAJU; MIRANDA; MUNDO NOVO; NAVIRAI; NIOAQUE; NOVA ALVORADA DO SUL; NOVA ANDRADINA; NOVO HORIZONTE DO SUL; PARAISO DAS AGUAS; PARANAIBA; PARANHOS; PEDRO GOMES; PONTA PORA; PORTO MURTINHO; RIBAS DO RIO PARDO; RIO BRILHANTE; RIO NEGRO; RIO VERDE DE MATO GROSSO; ROCHEDO; SANTA RITA DO PARDO; SAO GABRIEL DO OESTE; SETE QUEDAS; SELVIRIA; SIDROLANDIA; SONORA; TACURU; TAQUARUSSU; TERENOS; TRES LAGOAS; VICENTINA</t>
+  </si>
+  <si>
+    <t>500020; 500025; 500060; 500070; 500080; 500085; 500090; 500100; 500110; 500124; 500150; 500190; 500200; 500210; 500215; 500220; 500230; 500240; 500260; 500270; 500280; 500290; 500295; 500310; 500315; 500320; 500325; 500330; 500345; 500348; 500350; 500370; 500375; 500380; 500390; 500400; 500410; 500430; 500440; 500450; 500460; 500470; 500480; 500490; 500500; 500510; 500515; 500520; 500525; 500540; 500560; 500568; 500570; 500580; 500600; 500620; 500625; 500627; 500630; 500635; 500640; 500660; 500690; 500710; 500720; 500730; 500740; 500750; 500755; 500769; 500770; 500780; 500790; 500793; 500795; 500797; 500800; 500830; 500840</t>
+  </si>
+  <si>
+    <t>2839188</t>
   </si>
   <si>
     <t>ANGELICA CRISTINA SEGATTO CONGRO</t>
@@ -1068,7 +1044,7 @@
 Entre as estratégias, deverá ser organizado as cirurgias de forma a atender pacientes em filas eletivas das 03 regiões de saúde (Baixo Acre Purus, Alto Acre e Juruá) e deverá ser como base também, instrumentos de gestão, dados epidemiológicos da única macrorregião de saúde no Estado do Acre, controle social e outros. É importante destacar que as variáveis estão sujeitas a alterações, podendo ser consultadas.</t>
   </si>
   <si>
-    <t>Enviada para o MS</t>
+    <t>Reenviada para o MS</t>
   </si>
   <si>
     <t>ACRELANDIA; ASSIS BRASIL; BRASILEIA; BUJARI; CAPIXABA; CRUZEIRO DO SUL; EPITACIOLANDIA; FEIJO; JORDAO; MANCIO LIMA; MANOEL URBANO; MARECHAL THAUMATURGO; PLACIDO DE CASTRO; PORTO WALTER; RIO BRANCO; RODRIGUES ALVES; SANTA ROSA DO PURUS; SENADOR GUIOMARD; SENA MADUREIRA; TARAUACA; XAPURI; PORTO ACRE</t>
@@ -1078,6 +1054,15 @@
   </si>
   <si>
     <t>906876</t>
+  </si>
+  <si>
+    <t>PRAZO -  enviar ate 15/mar/2023  a planilha atendimento devidamente preenchida.</t>
+  </si>
+  <si>
+    <t>10/03/2023 18:51:15</t>
+  </si>
+  <si>
+    <t>2.550.776,40</t>
   </si>
   <si>
     <t>MONALISA RAFAELY ZAFFONATO DA ROSA</t>
@@ -1132,7 +1117,7 @@
 Após esse trâmite, é realizado novo contato com paciente para orientação e encaminhamentos para o procedimento cirúrgico conforme oferta de vaga.</t>
   </si>
   <si>
-    <t>plano-atendimento-perf-cir-eletiva-vrs-4a 07 03 2023 DEFINITIVO.xlsx</t>
+    <t>13.03 - plano-atendimento-perf-cir-eletiva-vrs-4a ACRE versao 3 diligências sanadas.xlsx</t>
   </si>
   <si>
     <t>plano-monitoramento-perf-cir-eletiva-vrs-3- DEFINITIVO.xlsx</t>
@@ -1253,6 +1238,12 @@
 6- A confirmação da execução (ou não) do procedimento cirúrgico somente ocorre após a finalização do mês autorizado, informação enviada pelas Unidades Executantes através dos meus oficiais (planilhas e chaves no SISREG) para o CRDF. Para os pacientes submetidos ao procedimento cirúrgico, a Unidade Executante realiza o fechamento da chave no SISREG, sinalizando na planilha oficial que o procedimento foi realizado. Para os pacientes não submetidos ao procedimento cirúrgico, a Unidade Executante deve fornecer justificativa (dentre as padronizadas na planilha oficial) para a não execução, bem como realizar a reinserção da solicitação no SISREG com a devida sinalização, sendo o paciente priorizado no próximo agendamento por se tratar de reautorização.</t>
   </si>
   <si>
+    <t>2023_03_13_plano-monitoramento-perf-cir-eletiva-vrs-3-1_DF.xlsx</t>
+  </si>
+  <si>
+    <t>2023_03_13_Plano_atendimento_perf_cir_eletiva_vrs_4a_DF.xlsx</t>
+  </si>
+  <si>
     <t>170640</t>
   </si>
   <si>
@@ -1281,15 +1272,14 @@
     <t>3289290</t>
   </si>
   <si>
-    <t>- Na planilha de atendimento que foi enviada, na aba ¿Execução¿, ficaram faltando os percentuais das parcelas mensais a serem executadas (cronograma), não é uma falha digna de se tornar uma diligência, mas é bom ser preenchida para não deixar nenhuma pendência. Importante salientar que a nova versão da planilha venha renomeada como ¿versão 2¿ e que a mesma não seja desbloqueada, pois ela é protegida devido a fórmulas existentes.
-- E por último, o procedimento laqueadura tubária (código SIGTAP 409060186) exige habilitação local, sendo assim é necessário que esta situação seja pactuada na CIB e regularizada junto ao CNES para evitar qualquer rejeição na produção.
-PRAZO PARA AJUSTE: 5 dias.</t>
+    <t>Orientamos que as unidades que possuem exigências de serviço e/ou habilitação e/ou leito devem ajustar o CNES antes de iniciar os atendimentos.
+O processo tramitará no SEI NUP 25000.033448/2023-35.</t>
   </si>
   <si>
     <t>CAROLINA PERES XAVIER PINTO</t>
   </si>
   <si>
-    <t>06/03/2023 17:53:17</t>
+    <t>10/03/2023 17:54:36</t>
   </si>
   <si>
     <t>9.251.808,75</t>
@@ -1307,9 +1297,6 @@
     <t>01/03/2023 14:31:35</t>
   </si>
   <si>
-    <t>05/04/2023</t>
-  </si>
-  <si>
     <t>JOÃO VICTOR DA SILVA BARBOZA</t>
   </si>
   <si>
@@ -1322,7 +1309,7 @@
     <t>joao.victor@saude.pi.gov.br // ducara@saude.pi.gov.br</t>
   </si>
   <si>
-    <t>CamScanner 03-01-2023 13.28.pdf</t>
+    <t>Resol cib quadro e projeto anexo.pdf</t>
   </si>
   <si>
     <t>008/2023</t>
@@ -1424,6 +1411,20 @@
     <t>4108508</t>
   </si>
   <si>
+    <t>Prazo: 5 dias.
+Orientamos para:
+1) Envio da CIB com a assinatura do COSEMS/ES;
+2) Envio da planilha de atendimento na versão 4a, devidamente preenchida; e
+3) Envio da planilha de monitoramento na versão 3.
+A apoiadora DRAC estará à disposição para quaisquer esclarecimentos complementares.</t>
+  </si>
+  <si>
+    <t>CLAUDIA RIBEIRO ZINI LISE</t>
+  </si>
+  <si>
+    <t>10/03/2023 17:20:19</t>
+  </si>
+  <si>
     <t>11.556.028,89</t>
   </si>
   <si>
@@ -1437,6 +1438,9 @@
   </si>
   <si>
     <t>09/03/2023 09:36:57</t>
+  </si>
+  <si>
+    <t>09/04/2023</t>
   </si>
   <si>
     <t>Maria Jose da Costa Mendes</t>
@@ -1684,7 +1688,22 @@
     <t>1815278</t>
   </si>
   <si>
+    <t>Existem exigências de SERVIÇO e/ou HABILITAÇÃO, orientamos para ajustar o CNES antes de iniciar os atendimentos.
+O estado informou que ajustará o CNES.
+A Planilha Atendimento aprovada, versão 4, corresponde à enviada por e-mail em 09/03/2023, a qual segue anexa.
+A proposta aprovada passará a tramitar pelo SEI NUP 25000.033366/2023-91.</t>
+  </si>
+  <si>
+    <t>LEANDRO ARANTES DE MELO</t>
+  </si>
+  <si>
+    <t>10/03/2023 15:59:43</t>
+  </si>
+  <si>
     <t>0,00</t>
+  </si>
+  <si>
+    <t>5.105.845,00</t>
   </si>
   <si>
     <t>MARIANA AGUIAR PRADO</t>
@@ -1908,6 +1927,17 @@
     <t>522357</t>
   </si>
   <si>
+    <t>Prazo para atendimento da diligência: 5 dias.
+Enquanto o Plano Estadual de Redução de Filas estiver sendo elaborado pode ser salvo para adequações, ainda no âmbito do Estado.
+Somente após a conclusão de todas as etapas do processo, deverá ser finalizado e enviado ao Ministério.</t>
+  </si>
+  <si>
+    <t>JANAINA LOPES DE NOVAIS</t>
+  </si>
+  <si>
+    <t>09/03/2023 16:25:51</t>
+  </si>
+  <si>
     <t>ELIELB VALES MACIEL</t>
   </si>
   <si>
@@ -1921,6 +1951,9 @@
   </si>
   <si>
     <t>09/03/2023 11:32:50</t>
+  </si>
+  <si>
+    <t>08/04/2023</t>
   </si>
   <si>
     <t>JUVANETE AMORAS TAVORA</t>
@@ -1975,6 +2008,54 @@
   </si>
   <si>
     <t>plano-atendimento-perf-cir-eletiva-vrs-4a.xlsx</t>
+  </si>
+  <si>
+    <t>170906</t>
+  </si>
+  <si>
+    <t>05.370.016/0001-00</t>
+  </si>
+  <si>
+    <t>FUNDO ESTADUAL DE SAUDE DO ESTADO RORAIMA</t>
+  </si>
+  <si>
+    <t>BOA VISTA</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>BOA VISTA; RORAINOPOLIS</t>
+  </si>
+  <si>
+    <t>140010; 140047</t>
+  </si>
+  <si>
+    <t>467978</t>
+  </si>
+  <si>
+    <t>ANA CLAUDIA ALMEIDA DE SOUZA</t>
+  </si>
+  <si>
+    <t>klaudia.souzza@gmail.com</t>
+  </si>
+  <si>
+    <t>95 81225490</t>
+  </si>
+  <si>
+    <t>07/06/2023</t>
+  </si>
+  <si>
+    <t>ANA CLÁUDIA ALMEIDA DE SOUZA</t>
+  </si>
+  <si>
+    <t>DIRETORA DE REGULAÇÃO</t>
+  </si>
+  <si>
+    <t>(95) 98122-5490</t>
+  </si>
+  <si>
+    <t>dereg.cgrac@saude.rr.gov.br</t>
   </si>
 </sst>
 </file>
@@ -4092,16 +4173,16 @@
         <v>183</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>123</v>
+        <v>184</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>87</v>
@@ -4122,13 +4203,13 @@
         <v>79</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="V8" s="2" t="s">
         <v>79</v>
@@ -4197,19 +4278,19 @@
         <v>79</v>
       </c>
       <c r="AR8" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AS8" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AT8" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AU8" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AV8" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AW8" s="2" t="s">
         <v>79</v>
@@ -4301,7 +4382,7 @@
     </row>
     <row r="9" spans="1:77">
       <c r="A9" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>76</v>
@@ -4322,10 +4403,10 @@
         <v>81</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>198</v>
@@ -4454,19 +4535,19 @@
         <v>79</v>
       </c>
       <c r="AZ9" s="2" t="s">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="BA9" s="2" t="s">
-        <v>79</v>
+        <v>209</v>
       </c>
       <c r="BB9" s="2" t="s">
-        <v>79</v>
+        <v>210</v>
       </c>
       <c r="BC9" s="2" t="s">
-        <v>79</v>
+        <v>211</v>
       </c>
       <c r="BD9" s="2" t="s">
-        <v>79</v>
+        <v>205</v>
       </c>
       <c r="BE9" s="2" t="s">
         <v>79</v>
@@ -4534,7 +4615,7 @@
     </row>
     <row r="10" spans="1:77">
       <c r="A10" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>76</v>
@@ -4555,19 +4636,19 @@
         <v>81</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>87</v>
@@ -4588,13 +4669,13 @@
         <v>79</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="V10" s="2" t="s">
         <v>79</v>
@@ -4663,19 +4744,19 @@
         <v>79</v>
       </c>
       <c r="AR10" s="2" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="AS10" s="2" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="AT10" s="2" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="AU10" s="2" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="AV10" s="2" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="AW10" s="2" t="s">
         <v>79</v>
@@ -4687,19 +4768,19 @@
         <v>79</v>
       </c>
       <c r="AZ10" s="2" t="s">
-        <v>212</v>
+        <v>79</v>
       </c>
       <c r="BA10" s="2" t="s">
-        <v>222</v>
+        <v>79</v>
       </c>
       <c r="BB10" s="2" t="s">
-        <v>223</v>
+        <v>79</v>
       </c>
       <c r="BC10" s="2" t="s">
-        <v>224</v>
+        <v>79</v>
       </c>
       <c r="BD10" s="2" t="s">
-        <v>218</v>
+        <v>79</v>
       </c>
       <c r="BE10" s="2" t="s">
         <v>79</v>
@@ -4767,7 +4848,7 @@
     </row>
     <row r="11" spans="1:77">
       <c r="A11" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>76</v>
@@ -4788,19 +4869,19 @@
         <v>81</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="L11" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>87</v>
@@ -4821,118 +4902,118 @@
         <v>79</v>
       </c>
       <c r="S11" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="T11" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="T11" s="2" t="s">
+      <c r="U11" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="U11" s="2" t="s">
+      <c r="V11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR11" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="V11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="W11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="X11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Y11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AE11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AH11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AJ11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AM11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AO11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AP11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AQ11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR11" s="2" t="s">
+      <c r="AS11" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="AS11" s="2" t="s">
+      <c r="AT11" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="AT11" s="2" t="s">
+      <c r="AU11" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="AV11" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="AW11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ11" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="BA11" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="AU11" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="AV11" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="AW11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AX11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AY11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AZ11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BA11" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="BB11" s="2" t="s">
-        <v>79</v>
+        <v>237</v>
       </c>
       <c r="BC11" s="2" t="s">
-        <v>79</v>
+        <v>238</v>
       </c>
       <c r="BD11" s="2" t="s">
-        <v>79</v>
+        <v>239</v>
       </c>
       <c r="BE11" s="2" t="s">
         <v>79</v>
@@ -5000,7 +5081,7 @@
     </row>
     <row r="12" spans="1:77">
       <c r="A12" s="2" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>76</v>
@@ -5021,19 +5102,19 @@
         <v>81</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>239</v>
+        <v>184</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>87</v>
@@ -5054,13 +5135,13 @@
         <v>79</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="V12" s="2" t="s">
         <v>79</v>
@@ -5087,10 +5168,10 @@
         <v>79</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>79</v>
+        <v>248</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>79</v>
+        <v>248</v>
       </c>
       <c r="AF12" s="2" t="s">
         <v>79</v>
@@ -5129,19 +5210,19 @@
         <v>79</v>
       </c>
       <c r="AR12" s="2" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="AS12" s="2" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="AT12" s="2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="AU12" s="2" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="AV12" s="2" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="AW12" s="2" t="s">
         <v>79</v>
@@ -5153,19 +5234,19 @@
         <v>79</v>
       </c>
       <c r="AZ12" s="2" t="s">
-        <v>241</v>
+        <v>79</v>
       </c>
       <c r="BA12" s="2" t="s">
-        <v>249</v>
+        <v>79</v>
       </c>
       <c r="BB12" s="2" t="s">
-        <v>250</v>
+        <v>79</v>
       </c>
       <c r="BC12" s="2" t="s">
-        <v>251</v>
+        <v>79</v>
       </c>
       <c r="BD12" s="2" t="s">
-        <v>252</v>
+        <v>79</v>
       </c>
       <c r="BE12" s="2" t="s">
         <v>79</v>
@@ -5233,7 +5314,7 @@
     </row>
     <row r="13" spans="1:77">
       <c r="A13" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>76</v>
@@ -5254,10 +5335,10 @@
         <v>81</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>255</v>
@@ -5269,7 +5350,7 @@
         <v>257</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>87</v>
+        <v>258</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>79</v>
@@ -5278,7 +5359,7 @@
         <v>79</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
       <c r="Q13" s="2" t="s">
         <v>88</v>
@@ -5287,13 +5368,13 @@
         <v>79</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="V13" s="2" t="s">
         <v>79</v>
@@ -5311,25 +5392,25 @@
         <v>79</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>79</v>
+        <v>262</v>
       </c>
       <c r="AB13" s="2" t="s">
-        <v>79</v>
+        <v>263</v>
       </c>
       <c r="AC13" s="2" t="s">
-        <v>79</v>
+        <v>264</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="AE13" s="2" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="AF13" s="2" t="s">
-        <v>79</v>
+        <v>265</v>
       </c>
       <c r="AG13" s="2" t="s">
-        <v>79</v>
+        <v>265</v>
       </c>
       <c r="AH13" s="2" t="s">
         <v>79</v>
@@ -5362,22 +5443,22 @@
         <v>79</v>
       </c>
       <c r="AR13" s="2" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="AS13" s="2" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="AT13" s="2" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="AU13" s="2" t="s">
-        <v>220</v>
+        <v>269</v>
       </c>
       <c r="AV13" s="2" t="s">
-        <v>221</v>
+        <v>79</v>
       </c>
       <c r="AW13" s="2" t="s">
-        <v>79</v>
+        <v>270</v>
       </c>
       <c r="AX13" s="2" t="s">
         <v>79</v>
@@ -5386,87 +5467,87 @@
         <v>79</v>
       </c>
       <c r="AZ13" s="2" t="s">
-        <v>79</v>
+        <v>256</v>
       </c>
       <c r="BA13" s="2" t="s">
-        <v>79</v>
+        <v>271</v>
       </c>
       <c r="BB13" s="2" t="s">
-        <v>79</v>
+        <v>272</v>
       </c>
       <c r="BC13" s="2" t="s">
-        <v>79</v>
+        <v>273</v>
       </c>
       <c r="BD13" s="2" t="s">
-        <v>79</v>
+        <v>274</v>
       </c>
       <c r="BE13" s="2" t="s">
-        <v>79</v>
+        <v>275</v>
       </c>
       <c r="BF13" s="2" t="s">
-        <v>79</v>
+        <v>276</v>
       </c>
       <c r="BG13" s="2" t="s">
-        <v>79</v>
+        <v>277</v>
       </c>
       <c r="BH13" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BI13" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BJ13" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BK13" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BL13" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BM13" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BN13" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BO13" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BP13" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BQ13" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BR13" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BS13" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BT13" s="2" t="s">
-        <v>79</v>
+        <v>278</v>
       </c>
       <c r="BU13" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BV13" s="2" t="s">
-        <v>79</v>
+        <v>279</v>
       </c>
       <c r="BW13" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BX13" s="2" t="s">
-        <v>79</v>
+        <v>280</v>
       </c>
       <c r="BY13" s="2" t="s">
-        <v>79</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:77">
       <c r="A14" s="2" t="s">
-        <v>265</v>
+        <v>282</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>76</v>
@@ -5487,22 +5568,22 @@
         <v>81</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>266</v>
+        <v>283</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>267</v>
+        <v>284</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>268</v>
+        <v>285</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>270</v>
+        <v>287</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>271</v>
+        <v>87</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>79</v>
@@ -5511,7 +5592,7 @@
         <v>79</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>88</v>
@@ -5520,13 +5601,13 @@
         <v>79</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>272</v>
+        <v>288</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
       <c r="V14" s="2" t="s">
         <v>79</v>
@@ -5544,25 +5625,25 @@
         <v>79</v>
       </c>
       <c r="AA14" s="2" t="s">
-        <v>275</v>
+        <v>79</v>
       </c>
       <c r="AB14" s="2" t="s">
-        <v>276</v>
+        <v>79</v>
       </c>
       <c r="AC14" s="2" t="s">
-        <v>277</v>
+        <v>79</v>
       </c>
       <c r="AD14" s="2" t="s">
-        <v>278</v>
+        <v>79</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>278</v>
+        <v>79</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>278</v>
+        <v>79</v>
       </c>
       <c r="AG14" s="2" t="s">
-        <v>278</v>
+        <v>79</v>
       </c>
       <c r="AH14" s="2" t="s">
         <v>79</v>
@@ -5595,22 +5676,22 @@
         <v>79</v>
       </c>
       <c r="AR14" s="2" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="AS14" s="2" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="AT14" s="2" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
       <c r="AU14" s="2" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="AV14" s="2" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="AW14" s="2" t="s">
-        <v>283</v>
+        <v>79</v>
       </c>
       <c r="AX14" s="2" t="s">
         <v>79</v>
@@ -5619,82 +5700,82 @@
         <v>79</v>
       </c>
       <c r="AZ14" s="2" t="s">
-        <v>269</v>
+        <v>79</v>
       </c>
       <c r="BA14" s="2" t="s">
-        <v>284</v>
+        <v>79</v>
       </c>
       <c r="BB14" s="2" t="s">
-        <v>285</v>
+        <v>79</v>
       </c>
       <c r="BC14" s="2" t="s">
-        <v>286</v>
+        <v>79</v>
       </c>
       <c r="BD14" s="2" t="s">
-        <v>287</v>
+        <v>79</v>
       </c>
       <c r="BE14" s="2" t="s">
-        <v>288</v>
+        <v>79</v>
       </c>
       <c r="BF14" s="2" t="s">
-        <v>289</v>
+        <v>79</v>
       </c>
       <c r="BG14" s="2" t="s">
-        <v>290</v>
+        <v>79</v>
       </c>
       <c r="BH14" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BI14" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BJ14" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BK14" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BL14" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BM14" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BN14" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BO14" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BP14" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BQ14" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BR14" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BS14" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BT14" s="2" t="s">
-        <v>291</v>
+        <v>79</v>
       </c>
       <c r="BU14" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BV14" s="2" t="s">
-        <v>292</v>
+        <v>79</v>
       </c>
       <c r="BW14" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BX14" s="2" t="s">
-        <v>293</v>
+        <v>79</v>
       </c>
       <c r="BY14" s="2" t="s">
-        <v>294</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:77">
@@ -5726,13 +5807,13 @@
         <v>297</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>184</v>
+        <v>298</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>185</v>
+        <v>299</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>87</v>
@@ -5753,13 +5834,13 @@
         <v>79</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>187</v>
+        <v>301</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>188</v>
+        <v>302</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>189</v>
+        <v>303</v>
       </c>
       <c r="V15" s="2" t="s">
         <v>79</v>
@@ -5828,43 +5909,43 @@
         <v>79</v>
       </c>
       <c r="AR15" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="AS15" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="AT15" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="AU15" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="AV15" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="AW15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AX15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ15" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="AS15" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="AT15" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="AU15" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="AV15" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="AW15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AX15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AY15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AZ15" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="BA15" s="2" t="s">
-        <v>79</v>
+        <v>309</v>
       </c>
       <c r="BB15" s="2" t="s">
-        <v>79</v>
+        <v>310</v>
       </c>
       <c r="BC15" s="2" t="s">
-        <v>79</v>
+        <v>311</v>
       </c>
       <c r="BD15" s="2" t="s">
-        <v>79</v>
+        <v>305</v>
       </c>
       <c r="BE15" s="2" t="s">
         <v>79</v>
@@ -5932,7 +6013,7 @@
     </row>
     <row r="16" spans="1:77">
       <c r="A16" s="2" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>76</v>
@@ -5953,22 +6034,22 @@
         <v>81</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>87</v>
+        <v>318</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>79</v>
@@ -5986,13 +6067,13 @@
         <v>79</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="V16" s="2" t="s">
         <v>79</v>
@@ -6010,13 +6091,13 @@
         <v>79</v>
       </c>
       <c r="AA16" s="2" t="s">
-        <v>79</v>
+        <v>322</v>
       </c>
       <c r="AB16" s="2" t="s">
-        <v>79</v>
+        <v>263</v>
       </c>
       <c r="AC16" s="2" t="s">
-        <v>79</v>
+        <v>323</v>
       </c>
       <c r="AD16" s="2" t="s">
         <v>79</v>
@@ -6025,10 +6106,10 @@
         <v>79</v>
       </c>
       <c r="AF16" s="2" t="s">
-        <v>79</v>
+        <v>324</v>
       </c>
       <c r="AG16" s="2" t="s">
-        <v>79</v>
+        <v>324</v>
       </c>
       <c r="AH16" s="2" t="s">
         <v>79</v>
@@ -6061,111 +6142,111 @@
         <v>79</v>
       </c>
       <c r="AR16" s="2" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="AS16" s="2" t="s">
-        <v>313</v>
+        <v>326</v>
       </c>
       <c r="AT16" s="2" t="s">
-        <v>314</v>
+        <v>327</v>
       </c>
       <c r="AU16" s="2" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="AV16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW16" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="AX16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ16" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="AW16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AX16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AY16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AZ16" s="2" t="s">
-        <v>307</v>
-      </c>
       <c r="BA16" s="2" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
       <c r="BB16" s="2" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="BC16" s="2" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
       <c r="BD16" s="2" t="s">
-        <v>313</v>
+        <v>332</v>
       </c>
       <c r="BE16" s="2" t="s">
-        <v>79</v>
+        <v>333</v>
       </c>
       <c r="BF16" s="2" t="s">
-        <v>79</v>
+        <v>334</v>
       </c>
       <c r="BG16" s="2" t="s">
-        <v>79</v>
+        <v>335</v>
       </c>
       <c r="BH16" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BI16" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BJ16" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BK16" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BL16" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BM16" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BN16" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BO16" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BP16" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BQ16" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BR16" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BS16" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BT16" s="2" t="s">
-        <v>79</v>
+        <v>336</v>
       </c>
       <c r="BU16" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BV16" s="2" t="s">
-        <v>79</v>
+        <v>337</v>
       </c>
       <c r="BW16" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BX16" s="2" t="s">
-        <v>79</v>
+        <v>338</v>
       </c>
       <c r="BY16" s="2" t="s">
-        <v>79</v>
+        <v>339</v>
       </c>
     </row>
     <row r="17" spans="1:77">
       <c r="A17" s="2" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>76</v>
@@ -6186,22 +6267,22 @@
         <v>81</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>321</v>
+        <v>341</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>325</v>
+        <v>345</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>326</v>
+        <v>87</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>79</v>
@@ -6210,7 +6291,7 @@
         <v>79</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
       <c r="Q17" s="2" t="s">
         <v>88</v>
@@ -6219,13 +6300,13 @@
         <v>79</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>327</v>
+        <v>346</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>328</v>
+        <v>347</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>329</v>
+        <v>348</v>
       </c>
       <c r="V17" s="2" t="s">
         <v>79</v>
@@ -6252,10 +6333,10 @@
         <v>79</v>
       </c>
       <c r="AD17" s="2" t="s">
-        <v>79</v>
+        <v>349</v>
       </c>
       <c r="AE17" s="2" t="s">
-        <v>79</v>
+        <v>349</v>
       </c>
       <c r="AF17" s="2" t="s">
         <v>79</v>
@@ -6294,22 +6375,22 @@
         <v>79</v>
       </c>
       <c r="AR17" s="2" t="s">
-        <v>330</v>
+        <v>350</v>
       </c>
       <c r="AS17" s="2" t="s">
-        <v>331</v>
+        <v>351</v>
       </c>
       <c r="AT17" s="2" t="s">
-        <v>332</v>
+        <v>352</v>
       </c>
       <c r="AU17" s="2" t="s">
-        <v>315</v>
+        <v>353</v>
       </c>
       <c r="AV17" s="2" t="s">
-        <v>79</v>
+        <v>354</v>
       </c>
       <c r="AW17" s="2" t="s">
-        <v>333</v>
+        <v>79</v>
       </c>
       <c r="AX17" s="2" t="s">
         <v>79</v>
@@ -6318,55 +6399,55 @@
         <v>79</v>
       </c>
       <c r="AZ17" s="2" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
       <c r="BA17" s="2" t="s">
-        <v>334</v>
+        <v>355</v>
       </c>
       <c r="BB17" s="2" t="s">
-        <v>335</v>
+        <v>356</v>
       </c>
       <c r="BC17" s="2" t="s">
-        <v>336</v>
+        <v>357</v>
       </c>
       <c r="BD17" s="2" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="BE17" s="2" t="s">
-        <v>338</v>
+        <v>79</v>
       </c>
       <c r="BF17" s="2" t="s">
-        <v>339</v>
+        <v>79</v>
       </c>
       <c r="BG17" s="2" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
       <c r="BH17" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BI17" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="BJ17" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="BK17" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="BL17" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="BM17" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="BN17" s="2" t="s">
         <v>161</v>
       </c>
       <c r="BO17" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="BP17" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="BP17" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="BQ17" s="2" t="s">
         <v>161</v>
@@ -6378,27 +6459,27 @@
         <v>161</v>
       </c>
       <c r="BT17" s="2" t="s">
-        <v>341</v>
+        <v>359</v>
       </c>
       <c r="BU17" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BV17" s="2" t="s">
-        <v>342</v>
+        <v>360</v>
       </c>
       <c r="BW17" s="2" t="s">
-        <v>79</v>
+        <v>361</v>
       </c>
       <c r="BX17" s="2" t="s">
-        <v>343</v>
+        <v>362</v>
       </c>
       <c r="BY17" s="2" t="s">
-        <v>344</v>
+        <v>363</v>
       </c>
     </row>
     <row r="18" spans="1:77">
       <c r="A18" s="2" t="s">
-        <v>345</v>
+        <v>364</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>76</v>
@@ -6419,22 +6500,22 @@
         <v>81</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>346</v>
+        <v>365</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>347</v>
+        <v>366</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>348</v>
+        <v>367</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>349</v>
+        <v>368</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>350</v>
+        <v>369</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>87</v>
+        <v>258</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>79</v>
@@ -6443,7 +6524,7 @@
         <v>79</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="Q18" s="2" t="s">
         <v>88</v>
@@ -6452,97 +6533,97 @@
         <v>79</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>351</v>
+        <v>370</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>352</v>
+        <v>371</v>
       </c>
       <c r="U18" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="AB18" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="AC18" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AD18" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="AE18" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="AF18" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="AG18" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="AH18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR18" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="AS18" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="AT18" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="AU18" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="V18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="W18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="X18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Y18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD18" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="AE18" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="AF18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AH18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AJ18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AM18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AO18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AP18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AQ18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR18" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="AS18" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="AT18" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="AU18" s="2" t="s">
-        <v>358</v>
-      </c>
       <c r="AV18" s="2" t="s">
-        <v>359</v>
+        <v>79</v>
       </c>
       <c r="AW18" s="2" t="s">
-        <v>79</v>
+        <v>380</v>
       </c>
       <c r="AX18" s="2" t="s">
         <v>79</v>
@@ -6551,43 +6632,43 @@
         <v>79</v>
       </c>
       <c r="AZ18" s="2" t="s">
-        <v>349</v>
+        <v>368</v>
       </c>
       <c r="BA18" s="2" t="s">
-        <v>360</v>
+        <v>381</v>
       </c>
       <c r="BB18" s="2" t="s">
-        <v>361</v>
+        <v>382</v>
       </c>
       <c r="BC18" s="2" t="s">
-        <v>362</v>
+        <v>383</v>
       </c>
       <c r="BD18" s="2" t="s">
-        <v>356</v>
+        <v>384</v>
       </c>
       <c r="BE18" s="2" t="s">
-        <v>79</v>
+        <v>385</v>
       </c>
       <c r="BF18" s="2" t="s">
-        <v>79</v>
+        <v>386</v>
       </c>
       <c r="BG18" s="2" t="s">
-        <v>363</v>
+        <v>387</v>
       </c>
       <c r="BH18" s="2" t="s">
-        <v>79</v>
+        <v>388</v>
       </c>
       <c r="BI18" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="BJ18" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="BK18" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="BL18" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="BM18" s="2" t="s">
         <v>161</v>
@@ -6599,7 +6680,7 @@
         <v>162</v>
       </c>
       <c r="BP18" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="BQ18" s="2" t="s">
         <v>161</v>
@@ -6608,30 +6689,30 @@
         <v>161</v>
       </c>
       <c r="BS18" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="BT18" s="2" t="s">
-        <v>364</v>
+        <v>389</v>
       </c>
       <c r="BU18" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BV18" s="2" t="s">
-        <v>365</v>
+        <v>390</v>
       </c>
       <c r="BW18" s="2" t="s">
-        <v>366</v>
+        <v>79</v>
       </c>
       <c r="BX18" s="2" t="s">
-        <v>79</v>
+        <v>391</v>
       </c>
       <c r="BY18" s="2" t="s">
-        <v>79</v>
+        <v>392</v>
       </c>
     </row>
     <row r="19" spans="1:77">
       <c r="A19" s="2" t="s">
-        <v>367</v>
+        <v>393</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>76</v>
@@ -6652,22 +6733,22 @@
         <v>81</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>368</v>
+        <v>394</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>369</v>
+        <v>184</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>370</v>
+        <v>395</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>371</v>
+        <v>396</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>372</v>
+        <v>86</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>139</v>
+        <v>87</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>79</v>
@@ -6685,13 +6766,13 @@
         <v>79</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>373</v>
+        <v>397</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>374</v>
+        <v>398</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>375</v>
+        <v>399</v>
       </c>
       <c r="V19" s="2" t="s">
         <v>79</v>
@@ -6709,25 +6790,25 @@
         <v>79</v>
       </c>
       <c r="AA19" s="2" t="s">
-        <v>376</v>
+        <v>79</v>
       </c>
       <c r="AB19" s="2" t="s">
-        <v>377</v>
+        <v>79</v>
       </c>
       <c r="AC19" s="2" t="s">
-        <v>378</v>
+        <v>79</v>
       </c>
       <c r="AD19" s="2" t="s">
-        <v>379</v>
+        <v>79</v>
       </c>
       <c r="AE19" s="2" t="s">
-        <v>379</v>
+        <v>79</v>
       </c>
       <c r="AF19" s="2" t="s">
-        <v>379</v>
+        <v>79</v>
       </c>
       <c r="AG19" s="2" t="s">
-        <v>379</v>
+        <v>79</v>
       </c>
       <c r="AH19" s="2" t="s">
         <v>79</v>
@@ -6760,111 +6841,111 @@
         <v>79</v>
       </c>
       <c r="AR19" s="2" t="s">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="AS19" s="2" t="s">
-        <v>381</v>
+        <v>401</v>
       </c>
       <c r="AT19" s="2" t="s">
-        <v>382</v>
+        <v>402</v>
       </c>
       <c r="AU19" s="2" t="s">
-        <v>358</v>
+        <v>403</v>
       </c>
       <c r="AV19" s="2" t="s">
-        <v>79</v>
+        <v>404</v>
       </c>
       <c r="AW19" s="2" t="s">
-        <v>383</v>
+        <v>79</v>
       </c>
       <c r="AX19" s="2" t="s">
         <v>79</v>
       </c>
       <c r="AY19" s="2" t="s">
-        <v>384</v>
+        <v>79</v>
       </c>
       <c r="AZ19" s="2" t="s">
-        <v>371</v>
+        <v>79</v>
       </c>
       <c r="BA19" s="2" t="s">
-        <v>385</v>
+        <v>79</v>
       </c>
       <c r="BB19" s="2" t="s">
-        <v>386</v>
+        <v>79</v>
       </c>
       <c r="BC19" s="2" t="s">
-        <v>387</v>
+        <v>79</v>
       </c>
       <c r="BD19" s="2" t="s">
-        <v>388</v>
+        <v>79</v>
       </c>
       <c r="BE19" s="2" t="s">
-        <v>389</v>
+        <v>79</v>
       </c>
       <c r="BF19" s="2" t="s">
-        <v>390</v>
+        <v>79</v>
       </c>
       <c r="BG19" s="2" t="s">
-        <v>391</v>
+        <v>79</v>
       </c>
       <c r="BH19" s="2" t="s">
-        <v>392</v>
+        <v>79</v>
       </c>
       <c r="BI19" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BJ19" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BK19" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BL19" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BM19" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BN19" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BO19" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BP19" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BQ19" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BR19" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BS19" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BT19" s="2" t="s">
-        <v>393</v>
+        <v>79</v>
       </c>
       <c r="BU19" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BV19" s="2" t="s">
-        <v>394</v>
+        <v>79</v>
       </c>
       <c r="BW19" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BX19" s="2" t="s">
-        <v>395</v>
+        <v>79</v>
       </c>
       <c r="BY19" s="2" t="s">
-        <v>396</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:77">
       <c r="A20" s="2" t="s">
-        <v>397</v>
+        <v>405</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>76</v>
@@ -6885,22 +6966,22 @@
         <v>81</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>398</v>
+        <v>406</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>197</v>
+        <v>407</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>86</v>
+        <v>410</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>87</v>
+        <v>139</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>79</v>
@@ -6909,7 +6990,7 @@
         <v>79</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
       <c r="Q20" s="2" t="s">
         <v>88</v>
@@ -6918,186 +6999,186 @@
         <v>79</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="U20" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="V20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA20" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="AB20" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="AC20" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="AD20" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="AE20" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="AF20" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="AG20" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="AH20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR20" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="AS20" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="AT20" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="AU20" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="V20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="W20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="X20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Y20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AE20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AH20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AJ20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AK20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AM20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AO20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AP20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AQ20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR20" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="AS20" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="AT20" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="AU20" s="2" t="s">
-        <v>407</v>
-      </c>
       <c r="AV20" s="2" t="s">
-        <v>408</v>
+        <v>79</v>
       </c>
       <c r="AW20" s="2" t="s">
-        <v>79</v>
+        <v>421</v>
       </c>
       <c r="AX20" s="2" t="s">
         <v>79</v>
       </c>
       <c r="AY20" s="2" t="s">
-        <v>79</v>
+        <v>422</v>
       </c>
       <c r="AZ20" s="2" t="s">
-        <v>79</v>
+        <v>409</v>
       </c>
       <c r="BA20" s="2" t="s">
-        <v>79</v>
+        <v>423</v>
       </c>
       <c r="BB20" s="2" t="s">
-        <v>79</v>
+        <v>424</v>
       </c>
       <c r="BC20" s="2" t="s">
-        <v>79</v>
+        <v>425</v>
       </c>
       <c r="BD20" s="2" t="s">
-        <v>79</v>
+        <v>426</v>
       </c>
       <c r="BE20" s="2" t="s">
-        <v>79</v>
+        <v>427</v>
       </c>
       <c r="BF20" s="2" t="s">
-        <v>79</v>
+        <v>428</v>
       </c>
       <c r="BG20" s="2" t="s">
-        <v>79</v>
+        <v>429</v>
       </c>
       <c r="BH20" s="2" t="s">
-        <v>79</v>
+        <v>430</v>
       </c>
       <c r="BI20" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BJ20" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BK20" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BL20" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BM20" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BN20" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BO20" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BP20" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BQ20" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BR20" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BS20" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BT20" s="2" t="s">
-        <v>79</v>
+        <v>431</v>
       </c>
       <c r="BU20" s="2" t="s">
-        <v>79</v>
+        <v>432</v>
       </c>
       <c r="BV20" s="2" t="s">
-        <v>79</v>
+        <v>433</v>
       </c>
       <c r="BW20" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BX20" s="2" t="s">
-        <v>79</v>
+        <v>434</v>
       </c>
       <c r="BY20" s="2" t="s">
-        <v>79</v>
+        <v>434</v>
       </c>
     </row>
     <row r="21" spans="1:77">
       <c r="A21" s="2" t="s">
-        <v>409</v>
+        <v>435</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>76</v>
@@ -7118,22 +7199,22 @@
         <v>81</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>410</v>
+        <v>436</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>411</v>
+        <v>184</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>412</v>
+        <v>437</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>413</v>
+        <v>438</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>414</v>
+        <v>439</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>326</v>
+        <v>87</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>79</v>
@@ -7151,13 +7232,13 @@
         <v>79</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>415</v>
+        <v>440</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>416</v>
+        <v>441</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>417</v>
+        <v>442</v>
       </c>
       <c r="V21" s="2" t="s">
         <v>79</v>
@@ -7184,10 +7265,10 @@
         <v>79</v>
       </c>
       <c r="AD21" s="2" t="s">
-        <v>418</v>
+        <v>443</v>
       </c>
       <c r="AE21" s="2" t="s">
-        <v>418</v>
+        <v>443</v>
       </c>
       <c r="AF21" s="2" t="s">
         <v>79</v>
@@ -7226,22 +7307,22 @@
         <v>79</v>
       </c>
       <c r="AR21" s="2" t="s">
-        <v>419</v>
+        <v>444</v>
       </c>
       <c r="AS21" s="2" t="s">
-        <v>420</v>
+        <v>445</v>
       </c>
       <c r="AT21" s="2" t="s">
-        <v>421</v>
+        <v>446</v>
       </c>
       <c r="AU21" s="2" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="AV21" s="2" t="s">
-        <v>79</v>
+        <v>404</v>
       </c>
       <c r="AW21" s="2" t="s">
-        <v>422</v>
+        <v>79</v>
       </c>
       <c r="AX21" s="2" t="s">
         <v>79</v>
@@ -7250,87 +7331,87 @@
         <v>79</v>
       </c>
       <c r="AZ21" s="2" t="s">
-        <v>413</v>
+        <v>79</v>
       </c>
       <c r="BA21" s="2" t="s">
-        <v>423</v>
+        <v>79</v>
       </c>
       <c r="BB21" s="2" t="s">
-        <v>424</v>
+        <v>79</v>
       </c>
       <c r="BC21" s="2" t="s">
-        <v>425</v>
+        <v>79</v>
       </c>
       <c r="BD21" s="2" t="s">
-        <v>426</v>
+        <v>79</v>
       </c>
       <c r="BE21" s="2" t="s">
-        <v>427</v>
+        <v>79</v>
       </c>
       <c r="BF21" s="2" t="s">
-        <v>428</v>
+        <v>79</v>
       </c>
       <c r="BG21" s="2" t="s">
-        <v>429</v>
+        <v>79</v>
       </c>
       <c r="BH21" s="2" t="s">
-        <v>430</v>
+        <v>79</v>
       </c>
       <c r="BI21" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BJ21" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BK21" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BL21" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BM21" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BN21" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BO21" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BP21" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BQ21" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BR21" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BS21" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BT21" s="2" t="s">
-        <v>431</v>
+        <v>79</v>
       </c>
       <c r="BU21" s="2" t="s">
-        <v>432</v>
+        <v>79</v>
       </c>
       <c r="BV21" s="2" t="s">
-        <v>433</v>
+        <v>79</v>
       </c>
       <c r="BW21" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BX21" s="2" t="s">
-        <v>434</v>
+        <v>79</v>
       </c>
       <c r="BY21" s="2" t="s">
-        <v>434</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:77">
       <c r="A22" s="2" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>76</v>
@@ -7351,19 +7432,19 @@
         <v>81</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>439</v>
+        <v>217</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>87</v>
@@ -7375,7 +7456,7 @@
         <v>79</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="Q22" s="2" t="s">
         <v>88</v>
@@ -7384,13 +7465,13 @@
         <v>79</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>440</v>
+        <v>451</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>441</v>
+        <v>452</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>442</v>
+        <v>453</v>
       </c>
       <c r="V22" s="2" t="s">
         <v>79</v>
@@ -7417,10 +7498,10 @@
         <v>79</v>
       </c>
       <c r="AD22" s="2" t="s">
-        <v>443</v>
+        <v>79</v>
       </c>
       <c r="AE22" s="2" t="s">
-        <v>443</v>
+        <v>79</v>
       </c>
       <c r="AF22" s="2" t="s">
         <v>79</v>
@@ -7459,19 +7540,19 @@
         <v>79</v>
       </c>
       <c r="AR22" s="2" t="s">
-        <v>444</v>
+        <v>454</v>
       </c>
       <c r="AS22" s="2" t="s">
-        <v>445</v>
+        <v>455</v>
       </c>
       <c r="AT22" s="2" t="s">
-        <v>446</v>
+        <v>456</v>
       </c>
       <c r="AU22" s="2" t="s">
-        <v>407</v>
+        <v>457</v>
       </c>
       <c r="AV22" s="2" t="s">
-        <v>408</v>
+        <v>458</v>
       </c>
       <c r="AW22" s="2" t="s">
         <v>79</v>
@@ -7563,7 +7644,7 @@
     </row>
     <row r="23" spans="1:77">
       <c r="A23" s="2" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>76</v>
@@ -7584,19 +7665,19 @@
         <v>81</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>230</v>
+        <v>463</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>87</v>
@@ -7617,13 +7698,13 @@
         <v>79</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>451</v>
+        <v>464</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>452</v>
+        <v>465</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>453</v>
+        <v>466</v>
       </c>
       <c r="V23" s="2" t="s">
         <v>79</v>
@@ -7692,13 +7773,13 @@
         <v>79</v>
       </c>
       <c r="AR23" s="2" t="s">
-        <v>454</v>
+        <v>467</v>
       </c>
       <c r="AS23" s="2" t="s">
-        <v>455</v>
+        <v>468</v>
       </c>
       <c r="AT23" s="2" t="s">
-        <v>456</v>
+        <v>469</v>
       </c>
       <c r="AU23" s="2" t="s">
         <v>457</v>
@@ -7716,73 +7797,73 @@
         <v>79</v>
       </c>
       <c r="AZ23" s="2" t="s">
-        <v>79</v>
+        <v>462</v>
       </c>
       <c r="BA23" s="2" t="s">
-        <v>79</v>
+        <v>470</v>
       </c>
       <c r="BB23" s="2" t="s">
-        <v>79</v>
+        <v>471</v>
       </c>
       <c r="BC23" s="2" t="s">
-        <v>79</v>
+        <v>472</v>
       </c>
       <c r="BD23" s="2" t="s">
-        <v>79</v>
+        <v>473</v>
       </c>
       <c r="BE23" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BF23" s="2" t="s">
-        <v>79</v>
+        <v>474</v>
       </c>
       <c r="BG23" s="2" t="s">
-        <v>79</v>
+        <v>475</v>
       </c>
       <c r="BH23" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BI23" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BJ23" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BK23" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BL23" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BM23" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BN23" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BO23" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BP23" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BQ23" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BR23" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BS23" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BT23" s="2" t="s">
-        <v>79</v>
+        <v>476</v>
       </c>
       <c r="BU23" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BV23" s="2" t="s">
-        <v>79</v>
+        <v>477</v>
       </c>
       <c r="BW23" s="2" t="s">
         <v>79</v>
@@ -7796,7 +7877,7 @@
     </row>
     <row r="24" spans="1:77">
       <c r="A24" s="2" t="s">
-        <v>459</v>
+        <v>478</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>76</v>
@@ -7817,19 +7898,19 @@
         <v>81</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>460</v>
+        <v>448</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>463</v>
+        <v>479</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>87</v>
@@ -7850,13 +7931,13 @@
         <v>79</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
       <c r="V24" s="2" t="s">
         <v>79</v>
@@ -7925,13 +8006,13 @@
         <v>79</v>
       </c>
       <c r="AR24" s="2" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="AS24" s="2" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="AT24" s="2" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
       <c r="AU24" s="2" t="s">
         <v>457</v>
@@ -7949,73 +8030,73 @@
         <v>79</v>
       </c>
       <c r="AZ24" s="2" t="s">
-        <v>462</v>
+        <v>79</v>
       </c>
       <c r="BA24" s="2" t="s">
-        <v>470</v>
+        <v>79</v>
       </c>
       <c r="BB24" s="2" t="s">
-        <v>471</v>
+        <v>79</v>
       </c>
       <c r="BC24" s="2" t="s">
-        <v>472</v>
+        <v>79</v>
       </c>
       <c r="BD24" s="2" t="s">
-        <v>473</v>
+        <v>79</v>
       </c>
       <c r="BE24" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BF24" s="2" t="s">
-        <v>474</v>
+        <v>79</v>
       </c>
       <c r="BG24" s="2" t="s">
-        <v>475</v>
+        <v>79</v>
       </c>
       <c r="BH24" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BI24" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BJ24" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BK24" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BL24" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BM24" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BN24" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BO24" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BP24" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BQ24" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BR24" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BS24" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BT24" s="2" t="s">
-        <v>476</v>
+        <v>79</v>
       </c>
       <c r="BU24" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BV24" s="2" t="s">
-        <v>477</v>
+        <v>79</v>
       </c>
       <c r="BW24" s="2" t="s">
         <v>79</v>
@@ -8029,7 +8110,7 @@
     </row>
     <row r="25" spans="1:77">
       <c r="A25" s="2" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>76</v>
@@ -8050,22 +8131,22 @@
         <v>81</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>448</v>
+        <v>481</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>449</v>
+        <v>482</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>450</v>
+        <v>483</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>87</v>
+        <v>258</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>79</v>
@@ -8074,7 +8155,7 @@
         <v>79</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
       <c r="Q25" s="2" t="s">
         <v>88</v>
@@ -8083,13 +8164,13 @@
         <v>79</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>451</v>
+        <v>485</v>
       </c>
       <c r="T25" s="2" t="s">
-        <v>452</v>
+        <v>486</v>
       </c>
       <c r="U25" s="2" t="s">
-        <v>453</v>
+        <v>487</v>
       </c>
       <c r="V25" s="2" t="s">
         <v>79</v>
@@ -8107,25 +8188,25 @@
         <v>79</v>
       </c>
       <c r="AA25" s="2" t="s">
-        <v>79</v>
+        <v>488</v>
       </c>
       <c r="AB25" s="2" t="s">
-        <v>79</v>
+        <v>489</v>
       </c>
       <c r="AC25" s="2" t="s">
-        <v>79</v>
+        <v>490</v>
       </c>
       <c r="AD25" s="2" t="s">
-        <v>79</v>
+        <v>491</v>
       </c>
       <c r="AE25" s="2" t="s">
-        <v>79</v>
+        <v>491</v>
       </c>
       <c r="AF25" s="2" t="s">
-        <v>79</v>
+        <v>492</v>
       </c>
       <c r="AG25" s="2" t="s">
-        <v>79</v>
+        <v>492</v>
       </c>
       <c r="AH25" s="2" t="s">
         <v>79</v>
@@ -8158,22 +8239,22 @@
         <v>79</v>
       </c>
       <c r="AR25" s="2" t="s">
-        <v>454</v>
+        <v>493</v>
       </c>
       <c r="AS25" s="2" t="s">
-        <v>455</v>
+        <v>494</v>
       </c>
       <c r="AT25" s="2" t="s">
-        <v>456</v>
+        <v>495</v>
       </c>
       <c r="AU25" s="2" t="s">
         <v>457</v>
       </c>
       <c r="AV25" s="2" t="s">
-        <v>458</v>
+        <v>79</v>
       </c>
       <c r="AW25" s="2" t="s">
-        <v>79</v>
+        <v>496</v>
       </c>
       <c r="AX25" s="2" t="s">
         <v>79</v>
@@ -8182,87 +8263,87 @@
         <v>79</v>
       </c>
       <c r="AZ25" s="2" t="s">
-        <v>79</v>
+        <v>483</v>
       </c>
       <c r="BA25" s="2" t="s">
-        <v>79</v>
+        <v>497</v>
       </c>
       <c r="BB25" s="2" t="s">
-        <v>79</v>
+        <v>498</v>
       </c>
       <c r="BC25" s="2" t="s">
-        <v>79</v>
+        <v>499</v>
       </c>
       <c r="BD25" s="2" t="s">
-        <v>79</v>
+        <v>500</v>
       </c>
       <c r="BE25" s="2" t="s">
-        <v>79</v>
+        <v>501</v>
       </c>
       <c r="BF25" s="2" t="s">
-        <v>79</v>
+        <v>502</v>
       </c>
       <c r="BG25" s="2" t="s">
-        <v>79</v>
+        <v>503</v>
       </c>
       <c r="BH25" s="2" t="s">
-        <v>79</v>
+        <v>504</v>
       </c>
       <c r="BI25" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BJ25" s="2" t="s">
-        <v>79</v>
+        <v>505</v>
       </c>
       <c r="BK25" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BL25" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BM25" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BN25" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BO25" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BP25" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BQ25" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BR25" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BS25" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BT25" s="2" t="s">
-        <v>79</v>
+        <v>506</v>
       </c>
       <c r="BU25" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BV25" s="2" t="s">
-        <v>79</v>
+        <v>507</v>
       </c>
       <c r="BW25" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BX25" s="2" t="s">
-        <v>79</v>
+        <v>508</v>
       </c>
       <c r="BY25" s="2" t="s">
-        <v>79</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:77">
       <c r="A26" s="2" t="s">
-        <v>480</v>
+        <v>509</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>76</v>
@@ -8283,22 +8364,22 @@
         <v>81</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>481</v>
+        <v>510</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>482</v>
+        <v>511</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>483</v>
+        <v>172</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>484</v>
+        <v>512</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>326</v>
+        <v>87</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>79</v>
@@ -8307,7 +8388,7 @@
         <v>79</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="Q26" s="2" t="s">
         <v>88</v>
@@ -8316,13 +8397,13 @@
         <v>79</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>485</v>
+        <v>513</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>486</v>
+        <v>514</v>
       </c>
       <c r="U26" s="2" t="s">
-        <v>487</v>
+        <v>515</v>
       </c>
       <c r="V26" s="2" t="s">
         <v>79</v>
@@ -8349,10 +8430,10 @@
         <v>79</v>
       </c>
       <c r="AD26" s="2" t="s">
-        <v>488</v>
+        <v>516</v>
       </c>
       <c r="AE26" s="2" t="s">
-        <v>488</v>
+        <v>516</v>
       </c>
       <c r="AF26" s="2" t="s">
         <v>79</v>
@@ -8391,22 +8472,22 @@
         <v>79</v>
       </c>
       <c r="AR26" s="2" t="s">
-        <v>489</v>
+        <v>517</v>
       </c>
       <c r="AS26" s="2" t="s">
-        <v>490</v>
+        <v>518</v>
       </c>
       <c r="AT26" s="2" t="s">
-        <v>491</v>
+        <v>519</v>
       </c>
       <c r="AU26" s="2" t="s">
-        <v>457</v>
+        <v>520</v>
       </c>
       <c r="AV26" s="2" t="s">
-        <v>79</v>
+        <v>521</v>
       </c>
       <c r="AW26" s="2" t="s">
-        <v>492</v>
+        <v>79</v>
       </c>
       <c r="AX26" s="2" t="s">
         <v>79</v>
@@ -8415,87 +8496,87 @@
         <v>79</v>
       </c>
       <c r="AZ26" s="2" t="s">
-        <v>483</v>
+        <v>79</v>
       </c>
       <c r="BA26" s="2" t="s">
-        <v>493</v>
+        <v>79</v>
       </c>
       <c r="BB26" s="2" t="s">
-        <v>494</v>
+        <v>79</v>
       </c>
       <c r="BC26" s="2" t="s">
-        <v>495</v>
+        <v>79</v>
       </c>
       <c r="BD26" s="2" t="s">
-        <v>496</v>
+        <v>79</v>
       </c>
       <c r="BE26" s="2" t="s">
-        <v>497</v>
+        <v>79</v>
       </c>
       <c r="BF26" s="2" t="s">
-        <v>498</v>
+        <v>79</v>
       </c>
       <c r="BG26" s="2" t="s">
-        <v>499</v>
+        <v>79</v>
       </c>
       <c r="BH26" s="2" t="s">
-        <v>500</v>
+        <v>79</v>
       </c>
       <c r="BI26" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BJ26" s="2" t="s">
-        <v>501</v>
+        <v>79</v>
       </c>
       <c r="BK26" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BL26" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BM26" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BN26" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BO26" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BP26" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BQ26" s="2" t="s">
-        <v>161</v>
+        <v>79</v>
       </c>
       <c r="BR26" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BS26" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BT26" s="2" t="s">
-        <v>502</v>
+        <v>79</v>
       </c>
       <c r="BU26" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BV26" s="2" t="s">
-        <v>503</v>
+        <v>79</v>
       </c>
       <c r="BW26" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BX26" s="2" t="s">
-        <v>504</v>
+        <v>79</v>
       </c>
       <c r="BY26" s="2" t="s">
-        <v>167</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:77">
       <c r="A27" s="2" t="s">
-        <v>505</v>
+        <v>522</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>76</v>
@@ -8516,19 +8597,19 @@
         <v>81</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>506</v>
+        <v>523</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>197</v>
+        <v>407</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>507</v>
+        <v>524</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>172</v>
+        <v>525</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>508</v>
+        <v>526</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>87</v>
@@ -8549,13 +8630,13 @@
         <v>79</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>509</v>
+        <v>527</v>
       </c>
       <c r="T27" s="2" t="s">
-        <v>510</v>
+        <v>528</v>
       </c>
       <c r="U27" s="2" t="s">
-        <v>511</v>
+        <v>529</v>
       </c>
       <c r="V27" s="2" t="s">
         <v>79</v>
@@ -8582,10 +8663,10 @@
         <v>79</v>
       </c>
       <c r="AD27" s="2" t="s">
-        <v>512</v>
+        <v>79</v>
       </c>
       <c r="AE27" s="2" t="s">
-        <v>512</v>
+        <v>79</v>
       </c>
       <c r="AF27" s="2" t="s">
         <v>79</v>
@@ -8624,19 +8705,19 @@
         <v>79</v>
       </c>
       <c r="AR27" s="2" t="s">
-        <v>513</v>
+        <v>530</v>
       </c>
       <c r="AS27" s="2" t="s">
-        <v>514</v>
+        <v>531</v>
       </c>
       <c r="AT27" s="2" t="s">
-        <v>515</v>
+        <v>532</v>
       </c>
       <c r="AU27" s="2" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="AV27" s="2" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="AW27" s="2" t="s">
         <v>79</v>
@@ -8728,7 +8809,7 @@
     </row>
     <row r="28" spans="1:77">
       <c r="A28" s="2" t="s">
-        <v>518</v>
+        <v>533</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>76</v>
@@ -8749,19 +8830,19 @@
         <v>81</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>519</v>
+        <v>534</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>411</v>
+        <v>314</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>520</v>
+        <v>535</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>521</v>
+        <v>536</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>522</v>
+        <v>537</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>87</v>
@@ -8782,13 +8863,13 @@
         <v>79</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>523</v>
+        <v>538</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>524</v>
+        <v>539</v>
       </c>
       <c r="U28" s="2" t="s">
-        <v>525</v>
+        <v>540</v>
       </c>
       <c r="V28" s="2" t="s">
         <v>79</v>
@@ -8857,19 +8938,19 @@
         <v>79</v>
       </c>
       <c r="AR28" s="2" t="s">
-        <v>526</v>
+        <v>541</v>
       </c>
       <c r="AS28" s="2" t="s">
-        <v>527</v>
+        <v>542</v>
       </c>
       <c r="AT28" s="2" t="s">
-        <v>528</v>
+        <v>543</v>
       </c>
       <c r="AU28" s="2" t="s">
-        <v>516</v>
+        <v>544</v>
       </c>
       <c r="AV28" s="2" t="s">
-        <v>517</v>
+        <v>545</v>
       </c>
       <c r="AW28" s="2" t="s">
         <v>79</v>
@@ -8961,7 +9042,7 @@
     </row>
     <row r="29" spans="1:77">
       <c r="A29" s="2" t="s">
-        <v>529</v>
+        <v>546</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>76</v>
@@ -8982,19 +9063,19 @@
         <v>81</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>530</v>
+        <v>448</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>322</v>
+        <v>184</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>531</v>
+        <v>449</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>532</v>
+        <v>450</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>533</v>
+        <v>547</v>
       </c>
       <c r="M29" s="2" t="s">
         <v>87</v>
@@ -9015,13 +9096,13 @@
         <v>79</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>534</v>
+        <v>451</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>535</v>
+        <v>452</v>
       </c>
       <c r="U29" s="2" t="s">
-        <v>536</v>
+        <v>453</v>
       </c>
       <c r="V29" s="2" t="s">
         <v>79</v>
@@ -9090,19 +9171,19 @@
         <v>79</v>
       </c>
       <c r="AR29" s="2" t="s">
-        <v>537</v>
+        <v>548</v>
       </c>
       <c r="AS29" s="2" t="s">
-        <v>538</v>
+        <v>549</v>
       </c>
       <c r="AT29" s="2" t="s">
-        <v>539</v>
+        <v>550</v>
       </c>
       <c r="AU29" s="2" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="AV29" s="2" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c r="AW29" s="2" t="s">
         <v>79</v>
@@ -9114,19 +9195,19 @@
         <v>79</v>
       </c>
       <c r="AZ29" s="2" t="s">
-        <v>79</v>
+        <v>450</v>
       </c>
       <c r="BA29" s="2" t="s">
-        <v>79</v>
+        <v>548</v>
       </c>
       <c r="BB29" s="2" t="s">
-        <v>79</v>
+        <v>551</v>
       </c>
       <c r="BC29" s="2" t="s">
-        <v>79</v>
+        <v>552</v>
       </c>
       <c r="BD29" s="2" t="s">
-        <v>79</v>
+        <v>549</v>
       </c>
       <c r="BE29" s="2" t="s">
         <v>79</v>
@@ -9194,7 +9275,7 @@
     </row>
     <row r="30" spans="1:77">
       <c r="A30" s="2" t="s">
-        <v>542</v>
+        <v>553</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>76</v>
@@ -9215,22 +9296,22 @@
         <v>81</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>448</v>
+        <v>554</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>449</v>
+        <v>555</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>450</v>
+        <v>556</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>543</v>
+        <v>557</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>87</v>
+        <v>139</v>
       </c>
       <c r="N30" s="2" t="s">
         <v>79</v>
@@ -9239,7 +9320,7 @@
         <v>79</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>79</v>
+        <v>140</v>
       </c>
       <c r="Q30" s="2" t="s">
         <v>88</v>
@@ -9248,13 +9329,13 @@
         <v>79</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>451</v>
+        <v>555</v>
       </c>
       <c r="T30" s="2" t="s">
-        <v>452</v>
+        <v>558</v>
       </c>
       <c r="U30" s="2" t="s">
-        <v>453</v>
+        <v>559</v>
       </c>
       <c r="V30" s="2" t="s">
         <v>79</v>
@@ -9272,25 +9353,25 @@
         <v>79</v>
       </c>
       <c r="AA30" s="2" t="s">
-        <v>79</v>
+        <v>560</v>
       </c>
       <c r="AB30" s="2" t="s">
-        <v>79</v>
+        <v>561</v>
       </c>
       <c r="AC30" s="2" t="s">
-        <v>79</v>
+        <v>562</v>
       </c>
       <c r="AD30" s="2" t="s">
-        <v>79</v>
+        <v>491</v>
       </c>
       <c r="AE30" s="2" t="s">
-        <v>79</v>
+        <v>491</v>
       </c>
       <c r="AF30" s="2" t="s">
-        <v>79</v>
+        <v>491</v>
       </c>
       <c r="AG30" s="2" t="s">
-        <v>79</v>
+        <v>491</v>
       </c>
       <c r="AH30" s="2" t="s">
         <v>79</v>
@@ -9323,111 +9404,111 @@
         <v>79</v>
       </c>
       <c r="AR30" s="2" t="s">
-        <v>544</v>
+        <v>563</v>
       </c>
       <c r="AS30" s="2" t="s">
-        <v>545</v>
+        <v>564</v>
       </c>
       <c r="AT30" s="2" t="s">
-        <v>546</v>
+        <v>565</v>
       </c>
       <c r="AU30" s="2" t="s">
-        <v>540</v>
+        <v>566</v>
       </c>
       <c r="AV30" s="2" t="s">
-        <v>541</v>
+        <v>79</v>
       </c>
       <c r="AW30" s="2" t="s">
-        <v>79</v>
+        <v>567</v>
       </c>
       <c r="AX30" s="2" t="s">
         <v>79</v>
       </c>
       <c r="AY30" s="2" t="s">
-        <v>79</v>
+        <v>568</v>
       </c>
       <c r="AZ30" s="2" t="s">
-        <v>450</v>
+        <v>556</v>
       </c>
       <c r="BA30" s="2" t="s">
-        <v>544</v>
+        <v>569</v>
       </c>
       <c r="BB30" s="2" t="s">
-        <v>547</v>
+        <v>570</v>
       </c>
       <c r="BC30" s="2" t="s">
-        <v>548</v>
+        <v>571</v>
       </c>
       <c r="BD30" s="2" t="s">
-        <v>545</v>
+        <v>572</v>
       </c>
       <c r="BE30" s="2" t="s">
-        <v>79</v>
+        <v>573</v>
       </c>
       <c r="BF30" s="2" t="s">
-        <v>79</v>
+        <v>574</v>
       </c>
       <c r="BG30" s="2" t="s">
-        <v>79</v>
+        <v>575</v>
       </c>
       <c r="BH30" s="2" t="s">
-        <v>79</v>
+        <v>576</v>
       </c>
       <c r="BI30" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BJ30" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BK30" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BL30" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BM30" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BN30" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BO30" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BP30" s="2" t="s">
-        <v>79</v>
+        <v>161</v>
       </c>
       <c r="BQ30" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BR30" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BS30" s="2" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="BT30" s="2" t="s">
-        <v>79</v>
+        <v>577</v>
       </c>
       <c r="BU30" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BV30" s="2" t="s">
-        <v>79</v>
+        <v>578</v>
       </c>
       <c r="BW30" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BX30" s="2" t="s">
-        <v>79</v>
+        <v>579</v>
       </c>
       <c r="BY30" s="2" t="s">
-        <v>79</v>
+        <v>580</v>
       </c>
     </row>
     <row r="31" spans="1:77">
       <c r="A31" s="2" t="s">
-        <v>549</v>
+        <v>581</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>76</v>
@@ -9448,22 +9529,22 @@
         <v>81</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>550</v>
+        <v>582</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>197</v>
+        <v>583</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>551</v>
+        <v>584</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>552</v>
+        <v>585</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>553</v>
+        <v>79</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>326</v>
+        <v>87</v>
       </c>
       <c r="N31" s="2" t="s">
         <v>79</v>
@@ -9472,7 +9553,7 @@
         <v>79</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="Q31" s="2" t="s">
         <v>88</v>
@@ -9481,13 +9562,13 @@
         <v>79</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>551</v>
+        <v>586</v>
       </c>
       <c r="T31" s="2" t="s">
-        <v>554</v>
+        <v>587</v>
       </c>
       <c r="U31" s="2" t="s">
-        <v>555</v>
+        <v>588</v>
       </c>
       <c r="V31" s="2" t="s">
         <v>79</v>
@@ -9514,10 +9595,10 @@
         <v>79</v>
       </c>
       <c r="AD31" s="2" t="s">
-        <v>488</v>
+        <v>79</v>
       </c>
       <c r="AE31" s="2" t="s">
-        <v>488</v>
+        <v>79</v>
       </c>
       <c r="AF31" s="2" t="s">
         <v>79</v>
@@ -9556,22 +9637,22 @@
         <v>79</v>
       </c>
       <c r="AR31" s="2" t="s">
-        <v>556</v>
+        <v>589</v>
       </c>
       <c r="AS31" s="2" t="s">
-        <v>557</v>
+        <v>590</v>
       </c>
       <c r="AT31" s="2" t="s">
-        <v>558</v>
+        <v>591</v>
       </c>
       <c r="AU31" s="2" t="s">
-        <v>559</v>
+        <v>566</v>
       </c>
       <c r="AV31" s="2" t="s">
-        <v>79</v>
+        <v>592</v>
       </c>
       <c r="AW31" s="2" t="s">
-        <v>560</v>
+        <v>79</v>
       </c>
       <c r="AX31" s="2" t="s">
         <v>79</v>
@@ -9580,37 +9661,37 @@
         <v>79</v>
       </c>
       <c r="AZ31" s="2" t="s">
-        <v>552</v>
+        <v>585</v>
       </c>
       <c r="BA31" s="2" t="s">
-        <v>561</v>
+        <v>593</v>
       </c>
       <c r="BB31" s="2" t="s">
-        <v>562</v>
+        <v>594</v>
       </c>
       <c r="BC31" s="2" t="s">
-        <v>563</v>
+        <v>595</v>
       </c>
       <c r="BD31" s="2" t="s">
-        <v>564</v>
+        <v>596</v>
       </c>
       <c r="BE31" s="2" t="s">
-        <v>565</v>
+        <v>79</v>
       </c>
       <c r="BF31" s="2" t="s">
-        <v>566</v>
+        <v>79</v>
       </c>
       <c r="BG31" s="2" t="s">
-        <v>567</v>
+        <v>79</v>
       </c>
       <c r="BH31" s="2" t="s">
-        <v>568</v>
+        <v>79</v>
       </c>
       <c r="BI31" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="BJ31" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BK31" s="2" t="s">
         <v>161</v>
@@ -9625,37 +9706,37 @@
         <v>161</v>
       </c>
       <c r="BO31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BP31" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="BQ31" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="BP31" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="BQ31" s="2" t="s">
-        <v>162</v>
-      </c>
       <c r="BR31" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BS31" s="2" t="s">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="BT31" s="2" t="s">
-        <v>569</v>
+        <v>79</v>
       </c>
       <c r="BU31" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BV31" s="2" t="s">
-        <v>570</v>
+        <v>79</v>
       </c>
       <c r="BW31" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BX31" s="2" t="s">
-        <v>571</v>
+        <v>79</v>
       </c>
       <c r="BY31" s="2" t="s">
-        <v>572</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>